<commit_message>
Updates to Pro_Genie to reduce combinatorial space
</commit_message>
<xml_diff>
--- a/progenieX/ProGenie_Parameters.xlsx
+++ b/progenieX/ProGenie_Parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\GitHub\MIT-BroadFoundry\progenieX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python27\MIT-BroadFoundry\progenieX\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="142">
   <si>
     <t>A</t>
   </si>
@@ -206,9 +206,6 @@
     <t>TTTTTTTTTTTTT</t>
   </si>
   <si>
-    <t>AAAAAAAAAAAAA</t>
-  </si>
-  <si>
     <t>TTAATTTAATTTT</t>
   </si>
   <si>
@@ -242,21 +239,12 @@
     <t>TTACCCGT</t>
   </si>
   <si>
-    <t>TCACCCGT</t>
-  </si>
-  <si>
     <t>CAGCCCTT</t>
   </si>
   <si>
-    <t>TTACCCGG</t>
-  </si>
-  <si>
     <t>ACACCCAAGCAT</t>
   </si>
   <si>
-    <t>ACACCTGGACAT</t>
-  </si>
-  <si>
     <t>ACCCCTTTTTTAC</t>
   </si>
   <si>
@@ -272,21 +260,12 @@
     <t>CGGCATCCA</t>
   </si>
   <si>
-    <t>CAGCTTCCT</t>
-  </si>
-  <si>
-    <t>CAACGGAAG</t>
-  </si>
-  <si>
     <t>ABF1 Choice Probabilities</t>
   </si>
   <si>
     <t>ABF1 Site Choices</t>
   </si>
   <si>
-    <t>AGCCGTAAATAGTTATCTTCCAAG</t>
-  </si>
-  <si>
     <t>ATCATCTATCACG</t>
   </si>
   <si>
@@ -450,14 +429,46 @@
   </si>
   <si>
     <t>TSS mutants are from consensus sequences in Lubliner et al.</t>
+  </si>
+  <si>
+    <t>Poly dA:dT Site Choice Probabilities</t>
+  </si>
+  <si>
+    <t>TTACCCGG*</t>
+  </si>
+  <si>
+    <t>*not inserted in this version due to combinatorial explosion</t>
+  </si>
+  <si>
+    <t>CAACGGAAG*</t>
+  </si>
+  <si>
+    <t>ACACCTGGACAT*</t>
+  </si>
+  <si>
+    <t>TCACCCGT*</t>
+  </si>
+  <si>
+    <t>CAGCTTCCT*</t>
+  </si>
+  <si>
+    <t>AGCCGTAAATAGTTATCTTCCAAG*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Trebuchet MS"/>
@@ -575,7 +586,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -701,11 +712,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -769,6 +791,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -829,6 +853,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1121,10 +1146,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="34"/>
+      <c r="A1" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1233,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1255,27 +1280,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="44" t="s">
+      <c r="A1" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="41" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>0</v>
@@ -1289,11 +1314,11 @@
       <c r="F2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="44"/>
-      <c r="H2" s="39"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="40" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1319,7 +1344,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="1" t="s">
         <v>33</v>
       </c>
@@ -1337,7 +1362,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="1" t="s">
         <v>34</v>
       </c>
@@ -1355,7 +1380,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="40" t="s">
         <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1375,7 +1400,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
@@ -1393,7 +1418,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1411,7 +1436,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="40" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1431,7 +1456,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1449,7 +1474,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="38"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
@@ -1467,7 +1492,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="40" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1487,7 +1512,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="38"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1505,7 +1530,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
@@ -1523,50 +1548,50 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="43"/>
+      <c r="B16" s="45"/>
       <c r="G16" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="35" t="s">
+      <c r="H17" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="36"/>
-      <c r="J17" s="35" t="s">
+      <c r="I17" s="38"/>
+      <c r="J17" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="36"/>
-      <c r="L17" s="35" t="s">
+      <c r="K17" s="38"/>
+      <c r="L17" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="M17" s="36"/>
-      <c r="N17" s="35" t="s">
+      <c r="M17" s="38"/>
+      <c r="N17" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="O17" s="36"/>
+      <c r="O17" s="38"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="38" t="s">
-        <v>99</v>
+      <c r="A18" s="40" t="s">
+        <v>92</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>32</v>
@@ -1579,47 +1604,47 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="J18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="L18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="N18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q18" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="R18" s="37"/>
+      <c r="Q18" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="R18" s="39"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="29">
-        <v>7</v>
-      </c>
-      <c r="D19" s="1">
-        <v>7</v>
+      <c r="C19" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="H19" s="1">
         <v>0.5</v>
@@ -1638,25 +1663,25 @@
       </c>
       <c r="O19" s="1"/>
       <c r="Q19" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="38"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="29">
-        <v>30</v>
-      </c>
-      <c r="D20" s="1">
-        <v>30</v>
+      <c r="C20" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="H20" s="1">
         <v>0.5</v>
@@ -1687,10 +1712,10 @@
         <v>0.1</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
@@ -1707,7 +1732,7 @@
         <v>92</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
@@ -1738,15 +1763,15 @@
         <v>0.5</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="38" t="s">
-        <v>104</v>
+      <c r="A22" s="40" t="s">
+        <v>97</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>34</v>
@@ -1758,7 +1783,7 @@
         <v>141</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
@@ -1789,22 +1814,22 @@
         <v>0.9</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="29">
-        <v>32</v>
-      </c>
-      <c r="D23" s="2">
-        <v>132</v>
+      <c r="C23" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
@@ -1814,100 +1839,100 @@
       <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="G25" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="H25" s="48"/>
-      <c r="I25" s="36"/>
+      <c r="A25" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="G25" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="H25" s="50"/>
+      <c r="I25" s="38"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="45" t="s">
-        <v>99</v>
+      <c r="A26" s="47" t="s">
+        <v>92</v>
       </c>
       <c r="B26" s="27">
         <v>0.25</v>
       </c>
       <c r="C26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="35" t="s">
+      <c r="H26" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="I26" s="36"/>
-      <c r="J26" s="35" t="s">
+      <c r="I26" s="38"/>
+      <c r="J26" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="36"/>
-      <c r="L26" s="35" t="s">
+      <c r="K26" s="38"/>
+      <c r="L26" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="M26" s="36"/>
-      <c r="N26" s="35" t="s">
+      <c r="M26" s="38"/>
+      <c r="N26" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="O26" s="36"/>
+      <c r="O26" s="38"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="46"/>
+      <c r="A27" s="48"/>
       <c r="B27" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C27" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="J27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="L27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M27" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="N27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q27" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="R27" s="36"/>
+      <c r="Q27" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="R27" s="38"/>
       <c r="T27" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="46"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C28" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D28" s="26">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="H28" s="1">
         <v>0.34</v>
@@ -1926,29 +1951,29 @@
       </c>
       <c r="O28" s="1"/>
       <c r="Q28" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="T28" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" s="46"/>
+      <c r="A29" s="48"/>
       <c r="B29" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C29" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D29" s="26">
         <f>SUM(C28:C29)</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="H29" s="1">
         <v>0.33</v>
@@ -1979,25 +2004,25 @@
         <v>0.1</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="R29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="T29" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A30" s="47"/>
+      <c r="A30" s="49"/>
       <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="H30" s="1">
         <v>0.33</v>
@@ -2028,18 +2053,18 @@
         <v>0.2</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="R30" s="1" t="s">
         <v>15</v>
       </c>
       <c r="T30" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A31" s="38" t="s">
-        <v>104</v>
+      <c r="A31" s="40" t="s">
+        <v>97</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>39</v>
@@ -2048,7 +2073,7 @@
         <v>0.95</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="H31" s="1">
         <v>0</v>
@@ -2079,14 +2104,14 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="38"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="1" t="s">
         <v>40</v>
       </c>
@@ -2094,29 +2119,29 @@
         <v>0.5</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="35" t="s">
+      <c r="H32" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="I32" s="36"/>
-      <c r="J32" s="35" t="s">
+      <c r="I32" s="38"/>
+      <c r="J32" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="K32" s="36"/>
-      <c r="L32" s="35" t="s">
+      <c r="K32" s="38"/>
+      <c r="L32" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="M32" s="36"/>
-      <c r="N32" s="35" t="s">
+      <c r="M32" s="38"/>
+      <c r="N32" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="O32" s="36"/>
-      <c r="Q32" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="R32" s="36"/>
+      <c r="O32" s="38"/>
+      <c r="Q32" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="R32" s="38"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="38"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="1" t="s">
         <v>41</v>
       </c>
@@ -2124,7 +2149,7 @@
         <v>0.25</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H33" s="1">
         <v>0.5</v>
@@ -2143,14 +2168,14 @@
       </c>
       <c r="O33" s="1"/>
       <c r="Q33" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="38"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="1" t="s">
         <v>42</v>
       </c>
@@ -2158,7 +2183,7 @@
         <v>0.67</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="H34" s="1">
         <v>0.5</v>
@@ -2189,22 +2214,22 @@
         <v>0.1</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="38"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C35" s="28">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="H35" s="1">
         <v>0</v>
@@ -2235,14 +2260,14 @@
         <v>0.5</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="40" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -2252,7 +2277,7 @@
         <v>0.67</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H36" s="1">
         <v>0</v>
@@ -2283,14 +2308,14 @@
         <v>0.9</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" s="38"/>
+      <c r="A37" s="40"/>
       <c r="B37" s="2" t="s">
         <v>40</v>
       </c>
@@ -2299,21 +2324,39 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A38" s="38"/>
+      <c r="A38" s="40"/>
       <c r="B38" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C38" s="28">
         <v>0.25</v>
       </c>
+      <c r="G38" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A39" s="38"/>
+      <c r="A39" s="40"/>
       <c r="B39" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C39" s="28">
         <v>0.67</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H39" s="2">
+        <v>1</v>
+      </c>
+      <c r="I39" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2356,10 +2399,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="H16" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2381,23 +2424,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="44" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="H1" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2412,11 +2455,11 @@
       <c r="D2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="39"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="41"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
@@ -2437,67 +2480,67 @@
       <c r="F3" s="14">
         <v>150</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="51"/>
+    </row>
+    <row r="4" spans="1:19" ht="33" x14ac:dyDescent="0.3">
+      <c r="H4" s="52"/>
+      <c r="I4" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="49"/>
-      <c r="M3" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3" s="49"/>
-    </row>
-    <row r="4" spans="1:19" ht="33" x14ac:dyDescent="0.3">
-      <c r="H4" s="50"/>
-      <c r="I4" s="21" t="s">
+      <c r="J4" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="20" t="s">
-        <v>64</v>
-      </c>
       <c r="K4" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="L4" s="20" t="s">
-        <v>64</v>
-      </c>
       <c r="M4" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="N4" s="20" t="s">
-        <v>64</v>
-      </c>
       <c r="O4" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="P4" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="P4" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="R4" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="S4" s="37"/>
+      <c r="R4" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="S4" s="39"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="37"/>
+      <c r="B5" s="39"/>
       <c r="H5" s="11">
         <v>1</v>
       </c>
       <c r="I5" s="2">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2">
@@ -2516,54 +2559,54 @@
         <v>1</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="37"/>
+      <c r="D6" s="39"/>
       <c r="H6" s="11">
         <v>2</v>
       </c>
       <c r="I6" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J6" s="5">
         <f>I6</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K6" s="2">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="L6" s="5">
         <f>K6</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="M6" s="2">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="N6" s="5">
         <f>M6</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="O6" s="2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P6" s="5">
         <f>O6</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="R6" s="1">
         <v>2</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>71</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -2584,38 +2627,38 @@
         <v>3</v>
       </c>
       <c r="I7" s="2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" ref="J7:P8" si="0">I7+J6</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="K7" s="2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="M7" s="2">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="O7" s="2">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="P7" s="5">
         <f t="shared" si="0"/>
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
       <c r="R7" s="1">
         <v>3</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -2623,7 +2666,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="4">
         <v>4</v>
@@ -2639,59 +2682,64 @@
       </c>
       <c r="J8" s="5">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="K8" s="2">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="M8" s="2">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="N8" s="5">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
       <c r="O8" s="2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P8" s="5">
         <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
+        <v>0.9</v>
       </c>
       <c r="R8" s="2">
         <v>4</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>73</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S9" s="55" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="H10" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
+      <c r="B10" s="39"/>
+      <c r="H10" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37" t="s">
+      <c r="B11" s="39"/>
+      <c r="C11" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="37"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
+      <c r="D11" s="39"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -2706,25 +2754,25 @@
       <c r="D12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="I12" s="49" t="s">
+      <c r="H12" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49" t="s">
+      <c r="J12" s="51"/>
+      <c r="K12" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="L12" s="49"/>
-      <c r="M12" s="49" t="s">
+      <c r="L12" s="51"/>
+      <c r="M12" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="N12" s="49"/>
-      <c r="O12" s="49" t="s">
+      <c r="N12" s="51"/>
+      <c r="O12" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="P12" s="49"/>
+      <c r="P12" s="51"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
@@ -2739,35 +2787,35 @@
       <c r="D13" s="16">
         <v>25</v>
       </c>
-      <c r="H13" s="50"/>
+      <c r="H13" s="52"/>
       <c r="I13" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="J13" s="20" t="s">
-        <v>67</v>
-      </c>
       <c r="K13" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="L13" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="L13" s="20" t="s">
-        <v>67</v>
-      </c>
       <c r="M13" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="N13" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="N13" s="20" t="s">
-        <v>67</v>
-      </c>
       <c r="O13" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="P13" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="P13" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="R13" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="S13" s="37"/>
+      <c r="R13" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="S13" s="39"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
@@ -2786,18 +2834,18 @@
         <v>1</v>
       </c>
       <c r="I14" s="2">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2">
-        <v>0.33</v>
+        <v>0.75</v>
       </c>
       <c r="L14" s="2">
         <f>K14</f>
-        <v>0.33</v>
+        <v>0.75</v>
       </c>
       <c r="M14" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2">
@@ -2808,7 +2856,7 @@
         <v>1</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -2828,46 +2876,46 @@
         <v>2</v>
       </c>
       <c r="I15" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J15" s="5">
         <f>I15</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="K15" s="2">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="L15" s="5">
         <f>K15</f>
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="M15" s="2">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="N15" s="5">
         <f>M15</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="O15" s="2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P15" s="5">
         <f>O15</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="R15" s="1">
         <v>2</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>75</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="16">
-        <v>130</v>
+      <c r="B16" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="C16" s="15">
         <v>125</v>
@@ -2879,28 +2927,28 @@
         <v>3</v>
       </c>
       <c r="I16" s="2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" ref="J16" si="1">I16+J15</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="K16" s="2">
-        <v>0.34</v>
+        <v>0.25</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" ref="L16" si="2">K16+L15</f>
-        <v>0.67</v>
+        <v>0.25</v>
       </c>
       <c r="M16" s="2">
         <v>0.5</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" ref="N16" si="3">M16+N15</f>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="O16" s="2">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="P16" s="5">
         <f t="shared" ref="P16" si="4">O16+P15</f>
@@ -2910,7 +2958,7 @@
         <v>3</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -2924,19 +2972,21 @@
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="R17" s="12"/>
-      <c r="S17" s="23"/>
+      <c r="S17" s="55" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="H18" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="H18" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
@@ -2952,9 +3002,9 @@
       <c r="E19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -2967,30 +3017,30 @@
         <v>1</v>
       </c>
       <c r="D20" s="3">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E20" s="3">
         <v>0.5</v>
       </c>
-      <c r="H20" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="I20" s="49" t="s">
+      <c r="H20" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49" t="s">
+      <c r="J20" s="51"/>
+      <c r="K20" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49" t="s">
+      <c r="L20" s="51"/>
+      <c r="M20" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="N20" s="49"/>
-      <c r="O20" s="49" t="s">
+      <c r="N20" s="51"/>
+      <c r="O20" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="P20" s="49"/>
+      <c r="P20" s="51"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
@@ -3008,50 +3058,50 @@
       <c r="E21" s="18">
         <v>0.1</v>
       </c>
-      <c r="H21" s="50"/>
+      <c r="H21" s="52"/>
       <c r="I21" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="J21" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="20" t="s">
-        <v>67</v>
-      </c>
       <c r="K21" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="L21" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="L21" s="20" t="s">
-        <v>67</v>
-      </c>
       <c r="M21" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="N21" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="N21" s="20" t="s">
-        <v>67</v>
-      </c>
       <c r="O21" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="P21" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="P21" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="R21" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="S21" s="37"/>
+      <c r="R21" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="S21" s="39"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H22" s="11">
         <v>1</v>
       </c>
       <c r="I22" s="2">
-        <v>0.34</v>
+        <v>0.9</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="L22" s="2"/>
       <c r="M22" s="2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2">
@@ -3062,24 +3112,24 @@
         <v>1</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
       <c r="H23" s="11">
         <v>2</v>
       </c>
       <c r="I23" s="2">
-        <v>0.33</v>
+        <v>0.1</v>
       </c>
       <c r="J23" s="5">
         <f>I23</f>
-        <v>0.33</v>
+        <v>0.1</v>
       </c>
       <c r="K23" s="2">
         <v>0.25</v>
@@ -3089,38 +3139,38 @@
         <v>0.25</v>
       </c>
       <c r="M23" s="2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="N23" s="5">
         <f>M23</f>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="O23" s="2">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="P23" s="5">
         <f>O23</f>
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="R23" s="1">
         <v>2</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52" t="s">
+      <c r="C24" s="53"/>
+      <c r="D24" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="52"/>
+      <c r="E24" s="54"/>
       <c r="H24" s="11">
         <v>3</v>
       </c>
@@ -3129,34 +3179,34 @@
       </c>
       <c r="J24" s="5">
         <f t="shared" ref="J24:J25" si="5">I24+J23</f>
-        <v>0.33</v>
+        <v>0.1</v>
       </c>
       <c r="K24" s="2">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="L24" s="5">
         <f t="shared" ref="L24:L25" si="6">K24+L23</f>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="M24" s="2">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="N24" s="5">
         <f t="shared" ref="N24:N25" si="7">M24+N23</f>
-        <v>0.60000000000000009</v>
+        <v>0.5</v>
       </c>
       <c r="O24" s="2">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="P24" s="5">
         <f t="shared" ref="P24:P25" si="8">O24+P23</f>
-        <v>0.79999999999999993</v>
+        <v>0.9</v>
       </c>
       <c r="R24" s="1">
         <v>3</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
@@ -3181,38 +3231,38 @@
         <v>4</v>
       </c>
       <c r="I25" s="1">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="J25" s="5">
         <f t="shared" si="5"/>
-        <v>0.66</v>
+        <v>0.1</v>
       </c>
       <c r="K25" s="2">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="L25" s="5">
         <f t="shared" si="6"/>
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="M25" s="2">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="N25" s="5">
         <f t="shared" si="7"/>
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="O25" s="2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P25" s="5">
         <f t="shared" si="8"/>
-        <v>0.89999999999999991</v>
+        <v>0.9</v>
       </c>
       <c r="R25" s="2">
         <v>4</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>82</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
@@ -3233,6 +3283,9 @@
         <f>E25+D26</f>
         <v>0.7</v>
       </c>
+      <c r="S26" s="55" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -3252,11 +3305,11 @@
         <f t="shared" ref="E27" si="10">E26+D27</f>
         <v>1</v>
       </c>
-      <c r="H27" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
+      <c r="H27" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -3275,9 +3328,9 @@
       <c r="E28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
@@ -3297,18 +3350,18 @@
         <v>36</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I29" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="J29" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="J29" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="R29" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="S29" s="37"/>
+      <c r="R29" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="S29" s="39"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -3331,14 +3384,14 @@
         <v>1</v>
       </c>
       <c r="I30" s="2">
-        <v>0.34</v>
+        <v>0</v>
       </c>
       <c r="J30" s="2"/>
       <c r="R30" s="1">
         <v>1</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
@@ -3346,41 +3399,41 @@
         <v>2</v>
       </c>
       <c r="I31" s="2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J31" s="5">
         <f>I31</f>
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R31" s="1">
         <v>2</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
       <c r="H32" s="11">
         <v>3</v>
       </c>
       <c r="I32" s="2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J32" s="5">
         <f t="shared" ref="J32" si="11">I32+J31</f>
-        <v>0.66</v>
+        <v>1</v>
       </c>
       <c r="R32" s="1">
         <v>3</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
@@ -3397,6 +3450,9 @@
       <c r="E33" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="S33" s="12" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
@@ -3414,11 +3470,11 @@
       <c r="E34" s="3">
         <v>0.1</v>
       </c>
-      <c r="H34" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="I34" s="38"/>
-      <c r="J34" s="38"/>
+      <c r="H34" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
@@ -3436,24 +3492,24 @@
       <c r="E35" s="18">
         <v>1</v>
       </c>
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="38"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H36" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I36" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="J36" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="J36" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="R36" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="S36" s="37"/>
+      <c r="R36" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="S36" s="39"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G37" s="22"/>
@@ -3468,7 +3524,7 @@
         <v>1</v>
       </c>
       <c r="S37" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
@@ -3487,7 +3543,7 @@
         <v>2</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
@@ -3495,15 +3551,15 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G40" s="23"/>
-      <c r="H40" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="I40" s="48"/>
-      <c r="J40" s="36"/>
-      <c r="R40" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="S40" s="36"/>
+      <c r="H40" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="I40" s="50"/>
+      <c r="J40" s="38"/>
+      <c r="R40" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="S40" s="38"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H41" s="11">
@@ -3519,40 +3575,40 @@
         <v>1</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="H43" s="35" t="s">
+      <c r="H43" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="I43" s="48"/>
-      <c r="J43" s="36"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="38"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H44" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I44" s="49" t="s">
+      <c r="I44" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="J44" s="49"/>
-      <c r="K44" s="49" t="s">
+      <c r="J44" s="51"/>
+      <c r="K44" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="L44" s="49"/>
-      <c r="M44" s="49" t="s">
+      <c r="L44" s="51"/>
+      <c r="M44" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="N44" s="49"/>
-      <c r="O44" s="49" t="s">
+      <c r="N44" s="51"/>
+      <c r="O44" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="P44" s="49"/>
-      <c r="R44" s="37" t="s">
+      <c r="P44" s="51"/>
+      <c r="R44" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="S44" s="37"/>
+      <c r="S44" s="39"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H45" s="1" t="s">
@@ -3566,31 +3622,31 @@
         <v>0</v>
       </c>
       <c r="K45" s="2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L45" s="6">
         <f>K45</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M45" s="2">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="N45" s="6">
         <f>M45</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="O45" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P45" s="6">
         <f>O45</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="R45" s="1" t="s">
         <v>54</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.3">
@@ -3598,38 +3654,38 @@
         <v>55</v>
       </c>
       <c r="I46" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J46" s="6">
         <f>I46+J45</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="K46" s="2">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="L46" s="6">
         <f>L45+K46</f>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="M46" s="2">
         <v>0.5</v>
       </c>
       <c r="N46" s="6">
         <f>N45+M46</f>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="O46" s="2">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="P46" s="6">
         <f>P45+O46</f>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="R46" s="1" t="s">
         <v>55</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.3">
@@ -3637,28 +3693,28 @@
         <v>53</v>
       </c>
       <c r="I47" s="2">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="J47" s="2">
         <f>I47+J46</f>
         <v>1</v>
       </c>
       <c r="K47" s="2">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="L47" s="2">
         <f t="shared" ref="L47" si="12">L46+K47</f>
         <v>1</v>
       </c>
       <c r="M47" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="N47" s="2">
         <f t="shared" ref="N47" si="13">N46+M47</f>
         <v>1</v>
       </c>
       <c r="O47" s="2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="P47" s="2">
         <f t="shared" ref="P47" si="14">P46+O47</f>
@@ -3670,6 +3726,61 @@
       <c r="S47" s="1" t="s">
         <v>58</v>
       </c>
+    </row>
+    <row r="49" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H49" s="34"/>
+      <c r="I49" s="34"/>
+      <c r="J49" s="34"/>
+      <c r="K49" s="33"/>
+      <c r="L49" s="33"/>
+      <c r="M49" s="33"/>
+      <c r="N49" s="33"/>
+      <c r="O49" s="33"/>
+      <c r="P49" s="33"/>
+    </row>
+    <row r="50" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H50" s="33"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="34"/>
+      <c r="L50" s="34"/>
+      <c r="M50" s="34"/>
+      <c r="N50" s="34"/>
+      <c r="O50" s="34"/>
+      <c r="P50" s="34"/>
+    </row>
+    <row r="51" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H51" s="33"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="33"/>
+      <c r="K51" s="33"/>
+      <c r="L51" s="33"/>
+      <c r="M51" s="33"/>
+      <c r="N51" s="33"/>
+      <c r="O51" s="33"/>
+      <c r="P51" s="33"/>
+    </row>
+    <row r="52" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H52" s="33"/>
+      <c r="I52" s="33"/>
+      <c r="J52" s="33"/>
+      <c r="K52" s="33"/>
+      <c r="L52" s="33"/>
+      <c r="M52" s="33"/>
+      <c r="N52" s="33"/>
+      <c r="O52" s="33"/>
+      <c r="P52" s="33"/>
+    </row>
+    <row r="53" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H53" s="33"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="33"/>
+      <c r="L53" s="33"/>
+      <c r="M53" s="33"/>
+      <c r="N53" s="33"/>
+      <c r="O53" s="33"/>
+      <c r="P53" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="47">
@@ -3722,6 +3833,7 @@
     <mergeCell ref="O12:P12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updates to many files
I got behind on my updating...
</commit_message>
<xml_diff>
--- a/progenieX/ProGenie_Parameters.xlsx
+++ b/progenieX/ProGenie_Parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15630" windowHeight="7080" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15630" windowHeight="7080"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="165">
   <si>
     <t>A</t>
   </si>
@@ -53,12 +53,6 @@
     <t>J6</t>
   </si>
   <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
     <t>GTGC</t>
   </si>
   <si>
@@ -86,12 +80,6 @@
     <t>GACC</t>
   </si>
   <si>
-    <t>BbsI</t>
-  </si>
-  <si>
-    <t>GCAGAAGACTA</t>
-  </si>
-  <si>
     <t>UAS Base Nucleotide Content</t>
   </si>
   <si>
@@ -311,9 +299,6 @@
     <t>Core Loc</t>
   </si>
   <si>
-    <t>Core Frag</t>
-  </si>
-  <si>
     <t>Frag Loc</t>
   </si>
   <si>
@@ -356,9 +341,6 @@
     <t>Dbl Sub</t>
   </si>
   <si>
-    <t>See UAS</t>
-  </si>
-  <si>
     <t>TSS Site Probability</t>
   </si>
   <si>
@@ -453,6 +435,93 @@
   </si>
   <si>
     <t>AGCCGTAAATAGTTATCTTCCAAG*</t>
+  </si>
+  <si>
+    <t>AAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>See below</t>
+  </si>
+  <si>
+    <t>Core-tbp</t>
+  </si>
+  <si>
+    <t>TATA (tbp sub-segment)</t>
+  </si>
+  <si>
+    <t>Kozak (utr sub-segment)</t>
+  </si>
+  <si>
+    <t>TSS         (tss sub-segment)</t>
+  </si>
+  <si>
+    <t>Core Sub</t>
+  </si>
+  <si>
+    <t>UAS1-F</t>
+  </si>
+  <si>
+    <t>UAS1-R</t>
+  </si>
+  <si>
+    <t>UAS2-F</t>
+  </si>
+  <si>
+    <t>UAS2-R</t>
+  </si>
+  <si>
+    <t>ACAT</t>
+  </si>
+  <si>
+    <t>Core-R</t>
+  </si>
+  <si>
+    <t>Core-F</t>
+  </si>
+  <si>
+    <t>Tolerance (%)</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>Core_F</t>
+  </si>
+  <si>
+    <t>Core_R</t>
+  </si>
+  <si>
+    <t>UAS1_F</t>
+  </si>
+  <si>
+    <t>UAS1_R</t>
+  </si>
+  <si>
+    <t>UAS2_F</t>
+  </si>
+  <si>
+    <t>UAS2_R</t>
+  </si>
+  <si>
+    <t>TGTGCGGAAGACTT</t>
+  </si>
+  <si>
+    <t>TGGCGAGAAGACCA</t>
+  </si>
+  <si>
+    <t>TCCCCAGAAGACGT</t>
+  </si>
+  <si>
+    <t>TGCGTGGAAGACTA</t>
+  </si>
+  <si>
+    <t>TCTTGCGAAGACTA</t>
+  </si>
+  <si>
+    <t>TGCTGGGAAGACTA</t>
   </si>
 </sst>
 </file>
@@ -586,7 +655,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -723,11 +792,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -793,10 +884,15 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -805,8 +901,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -830,13 +932,13 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -853,7 +955,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1130,10 +1232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A4:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1141,35 +1243,34 @@
     <col min="1" max="1" width="7.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="36"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="39"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G5" s="60" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1177,7 +1278,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="60" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1185,7 +1295,16 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" s="60" t="s">
+        <v>161</v>
       </c>
       <c r="J7" s="12"/>
     </row>
@@ -1194,7 +1313,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G8" s="60" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1202,7 +1330,16 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="60" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1210,44 +1347,53 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>146</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G10" s="60" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>18</v>
+      <c r="B16" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1256,10 +1402,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T39"/>
+  <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1276,53 +1422,53 @@
     <col min="14" max="14" width="4.625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4.875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="41" t="s">
-        <v>26</v>
+      <c r="A1" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="51" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="41"/>
+        <v>20</v>
+      </c>
+      <c r="G2" s="51"/>
+      <c r="H2" s="46"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
-        <v>39</v>
+      <c r="A3" s="45" t="s">
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C3" s="25">
         <v>30</v>
@@ -1342,11 +1488,14 @@
       <c r="H3" s="14">
         <v>50</v>
       </c>
+      <c r="I3" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C4" s="25">
         <v>24</v>
@@ -1360,11 +1509,20 @@
       <c r="F4" s="10">
         <v>10</v>
       </c>
+      <c r="G4" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="H4" s="14">
+        <v>50</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C5" s="25">
         <v>40</v>
@@ -1378,13 +1536,22 @@
       <c r="F5" s="10">
         <v>16</v>
       </c>
+      <c r="G5" s="14">
+        <v>5</v>
+      </c>
+      <c r="H5" s="14">
+        <v>26</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
-        <v>40</v>
+      <c r="A6" s="45" t="s">
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C6" s="25">
         <v>32</v>
@@ -1400,9 +1567,9 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C7" s="25">
         <v>32</v>
@@ -1418,9 +1585,9 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="40"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8" s="25">
         <v>44</v>
@@ -1436,11 +1603,11 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
-        <v>41</v>
+      <c r="A9" s="45" t="s">
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C9" s="25">
         <v>36</v>
@@ -1456,9 +1623,9 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10" s="25">
         <v>34</v>
@@ -1474,9 +1641,9 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C11" s="25">
         <v>36</v>
@@ -1492,11 +1659,11 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="40" t="s">
-        <v>42</v>
+      <c r="A12" s="45" t="s">
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C12" s="25">
         <v>34</v>
@@ -1512,9 +1679,9 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="40"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C13" s="25">
         <v>36</v>
@@ -1530,9 +1697,9 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="40"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C14" s="25">
         <v>30</v>
@@ -1548,53 +1715,53 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="45"/>
+      <c r="A16" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="50"/>
       <c r="G16" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="38"/>
-      <c r="J17" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="K17" s="38"/>
-      <c r="L17" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="M17" s="38"/>
-      <c r="N17" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="O17" s="38"/>
+      <c r="H17" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="41"/>
+      <c r="J17" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="41"/>
+      <c r="L17" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="M17" s="41"/>
+      <c r="N17" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="O17" s="41"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="40" t="s">
-        <v>92</v>
+      <c r="A18" s="45" t="s">
+        <v>88</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C18" s="29">
         <v>2</v>
@@ -1604,47 +1771,47 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="Q18" s="39" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="R18" s="39"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
+      <c r="A19" s="45"/>
       <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>36</v>
-      </c>
       <c r="D19" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H19" s="1">
         <v>0.5</v>
@@ -1663,25 +1830,25 @@
       </c>
       <c r="O19" s="1"/>
       <c r="Q19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="R19" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="R19" s="1" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="40"/>
+      <c r="A20" s="45"/>
       <c r="B20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="29" t="s">
-        <v>36</v>
-      </c>
       <c r="D20" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H20" s="1">
         <v>0.5</v>
@@ -1712,18 +1879,18 @@
         <v>0.1</v>
       </c>
       <c r="Q20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="R20" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="R20" s="1" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>33</v>
+      <c r="A21" s="35" t="s">
+        <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C21" s="29">
         <v>42</v>
@@ -1732,7 +1899,7 @@
         <v>92</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
@@ -1763,27 +1930,27 @@
         <v>0.5</v>
       </c>
       <c r="Q21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R21" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="R21" s="1" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="29">
+        <v>17</v>
+      </c>
+      <c r="D22" s="1">
+        <v>117</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="29">
-        <v>41</v>
-      </c>
-      <c r="D22" s="1">
-        <v>141</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
@@ -1814,22 +1981,22 @@
         <v>0.9</v>
       </c>
       <c r="Q22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="R22" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="R22" s="1" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="40"/>
+      <c r="A23" s="45"/>
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
@@ -1840,90 +2007,90 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="39" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
-      <c r="G25" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="H25" s="50"/>
-      <c r="I25" s="38"/>
+      <c r="G25" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="H25" s="55"/>
+      <c r="I25" s="41"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="47" t="s">
-        <v>92</v>
+      <c r="A26" s="52" t="s">
+        <v>139</v>
       </c>
       <c r="B26" s="27">
         <v>0.25</v>
       </c>
       <c r="C26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="I26" s="38"/>
-      <c r="J26" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="K26" s="38"/>
-      <c r="L26" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="M26" s="38"/>
-      <c r="N26" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="O26" s="38"/>
+      <c r="H26" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="I26" s="41"/>
+      <c r="J26" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" s="41"/>
+      <c r="L26" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="M26" s="41"/>
+      <c r="N26" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="O26" s="41"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="48"/>
+      <c r="A27" s="53"/>
       <c r="B27" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q27" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="R27" s="38"/>
+        <v>62</v>
+      </c>
+      <c r="Q27" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="R27" s="41"/>
       <c r="T27" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="48"/>
+      <c r="A28" s="53"/>
       <c r="B28" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
@@ -1932,7 +2099,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="H28" s="1">
         <v>0.34</v>
@@ -1951,19 +2118,19 @@
       </c>
       <c r="O28" s="1"/>
       <c r="Q28" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="T28" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" s="48"/>
+      <c r="A29" s="53"/>
       <c r="B29" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
@@ -1973,7 +2140,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H29" s="1">
         <v>0.33</v>
@@ -2004,25 +2171,25 @@
         <v>0.1</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="T29" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A30" s="49"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H30" s="1">
         <v>0.33</v>
@@ -2053,27 +2220,27 @@
         <v>0.2</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="T30" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A31" s="40" t="s">
-        <v>97</v>
+      <c r="A31" s="44" t="s">
+        <v>140</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C31" s="28">
         <v>0.95</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H31" s="1">
         <v>0</v>
@@ -2104,52 +2271,52 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="40"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C32" s="28">
         <v>0.5</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="I32" s="38"/>
-      <c r="J32" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="K32" s="38"/>
-      <c r="L32" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="M32" s="38"/>
-      <c r="N32" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="O32" s="38"/>
-      <c r="Q32" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="R32" s="38"/>
+      <c r="H32" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32" s="41"/>
+      <c r="J32" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="K32" s="41"/>
+      <c r="L32" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="M32" s="41"/>
+      <c r="N32" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="O32" s="41"/>
+      <c r="Q32" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="R32" s="41"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="40"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C33" s="28">
         <v>0.25</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H33" s="1">
         <v>0.5</v>
@@ -2168,22 +2335,22 @@
       </c>
       <c r="O33" s="1"/>
       <c r="Q33" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="40"/>
+      <c r="A34" s="44"/>
       <c r="B34" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C34" s="28">
         <v>0.67</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="H34" s="1">
         <v>0.5</v>
@@ -2214,22 +2381,22 @@
         <v>0.1</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="40"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C35" s="28">
         <v>0</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H35" s="1">
         <v>0</v>
@@ -2260,24 +2427,24 @@
         <v>0.5</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="40" t="s">
-        <v>33</v>
+      <c r="A36" s="44" t="s">
+        <v>141</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C36" s="28">
         <v>0.67</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H36" s="1">
         <v>0</v>
@@ -2308,70 +2475,192 @@
         <v>0.9</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" s="40"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C37" s="28">
         <v>0.5</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A38" s="40"/>
+      <c r="A38" s="44"/>
       <c r="B38" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C38" s="28">
         <v>0.25</v>
       </c>
       <c r="G38" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A39" s="40"/>
+      <c r="A39" s="44"/>
       <c r="B39" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C39" s="28">
         <v>0.67</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="I39" s="43"/>
+      <c r="J39" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="K39" s="43"/>
+      <c r="L39" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="M39" s="43"/>
+      <c r="N39" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="O39" s="43"/>
+      <c r="Q39" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="R39" s="41"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1">
+        <v>0</v>
+      </c>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1">
+        <v>0</v>
+      </c>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1">
+        <v>0</v>
+      </c>
+      <c r="O40" s="1"/>
+      <c r="Q40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H41" s="38">
+        <v>0.25</v>
+      </c>
+      <c r="I41" s="38"/>
+      <c r="J41" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K41" s="38"/>
+      <c r="L41" s="38">
+        <v>0.75</v>
+      </c>
+      <c r="M41" s="38"/>
+      <c r="N41" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="O41" s="38"/>
+      <c r="Q41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R41" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H39" s="2">
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H42" s="38">
+        <v>0.75</v>
+      </c>
+      <c r="I42" s="38"/>
+      <c r="J42" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="K42" s="38"/>
+      <c r="L42" s="38">
+        <v>0.25</v>
+      </c>
+      <c r="M42" s="38"/>
+      <c r="N42" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="O42" s="38"/>
+      <c r="Q42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A44" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46" s="3">
         <v>1</v>
       </c>
-      <c r="I39" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="R39" s="1" t="s">
-        <v>59</v>
+      <c r="C46" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="36">
+    <mergeCell ref="N26:O26"/>
     <mergeCell ref="Q27:R27"/>
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="J32:K32"/>
     <mergeCell ref="L32:M32"/>
     <mergeCell ref="N32:O32"/>
     <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:O26"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A31:A35"/>
     <mergeCell ref="A26:A30"/>
@@ -2379,6 +2668,9 @@
     <mergeCell ref="L17:M17"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="G25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
     <mergeCell ref="N17:O17"/>
     <mergeCell ref="Q18:R18"/>
     <mergeCell ref="A18:A20"/>
@@ -2391,6 +2683,13 @@
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="A36:A39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2401,8 +2700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H16" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2424,116 +2723,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
+      <c r="F1" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="41"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
+        <v>20</v>
+      </c>
+      <c r="E2" s="51"/>
+      <c r="F2" s="46"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="8">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C3" s="9">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D3" s="10">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E3" s="14">
-        <v>1E-3</v>
+        <v>2</v>
       </c>
       <c r="F3" s="14">
-        <v>150</v>
-      </c>
-      <c r="H3" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3" s="51"/>
+        <v>126</v>
+      </c>
+      <c r="H3" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="56"/>
     </row>
     <row r="4" spans="1:19" ht="33" x14ac:dyDescent="0.3">
-      <c r="H4" s="52"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J4" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4" s="39" t="s">
         <v>63</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="M4" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="N4" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="O4" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="P4" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="R4" s="39" t="s">
-        <v>67</v>
       </c>
       <c r="S4" s="39"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="39" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B5" s="39"/>
       <c r="H5" s="11">
@@ -2559,16 +2858,16 @@
         <v>1</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="39" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" s="39"/>
       <c r="C6" s="39" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D6" s="39"/>
       <c r="H6" s="11">
@@ -2606,21 +2905,21 @@
         <v>2</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F7" s="12"/>
       <c r="H7" s="11">
@@ -2658,7 +2957,7 @@
         <v>3</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -2709,126 +3008,126 @@
         <v>4</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="S9" s="55" t="s">
-        <v>136</v>
+      <c r="S9" s="37" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="39" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B10" s="39"/>
-      <c r="H10" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
+      <c r="H10" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="39" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B11" s="39"/>
       <c r="C11" s="39" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D11" s="39"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="P12" s="51"/>
+        <v>27</v>
+      </c>
+      <c r="H12" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="P12" s="56"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B13" s="16">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C13" s="15">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D13" s="16">
-        <v>25</v>
-      </c>
-      <c r="H13" s="52"/>
+        <v>20</v>
+      </c>
+      <c r="H13" s="57"/>
       <c r="I13" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L13" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O13" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="P13" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="R13" s="39" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="S13" s="39"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B14" s="16">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C14" s="15">
-        <v>60</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>36</v>
+        <v>50</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0</v>
       </c>
       <c r="H14" s="11">
         <v>1</v>
@@ -2856,21 +3155,21 @@
         <v>1</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>36</v>
+      <c r="A15" s="17">
+        <v>0</v>
       </c>
       <c r="B15" s="16">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C15" s="15">
-        <v>95</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>36</v>
+        <v>75</v>
+      </c>
+      <c r="D15" s="17">
+        <v>0</v>
       </c>
       <c r="H15" s="11">
         <v>2</v>
@@ -2907,21 +3206,21 @@
         <v>2</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>36</v>
+      <c r="A16" s="17">
+        <v>0</v>
+      </c>
+      <c r="B16" s="36">
+        <v>0</v>
       </c>
       <c r="C16" s="15">
-        <v>125</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>36</v>
+        <v>105</v>
+      </c>
+      <c r="D16" s="17">
+        <v>0</v>
       </c>
       <c r="H16" s="11">
         <v>3</v>
@@ -2958,7 +3257,7 @@
         <v>3</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -2972,43 +3271,43 @@
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="R17" s="12"/>
-      <c r="S17" s="55" t="s">
-        <v>136</v>
+      <c r="S17" s="37" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="H18" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="A18" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="H18" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
+        <v>38</v>
+      </c>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -3022,29 +3321,29 @@
       <c r="E20" s="3">
         <v>0.5</v>
       </c>
-      <c r="H20" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="I20" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="N20" s="51"/>
-      <c r="O20" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="P20" s="51"/>
+      <c r="H20" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="56"/>
+      <c r="K20" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="L20" s="56"/>
+      <c r="M20" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="N20" s="56"/>
+      <c r="O20" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="P20" s="56"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B21" s="18">
         <v>1</v>
@@ -3058,33 +3357,33 @@
       <c r="E21" s="18">
         <v>0.1</v>
       </c>
-      <c r="H21" s="52"/>
+      <c r="H21" s="57"/>
       <c r="I21" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K21" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L21" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="M21" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="P21" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="R21" s="39" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="S21" s="39"/>
     </row>
@@ -3112,12 +3411,12 @@
         <v>1</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="39" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
@@ -3156,21 +3455,21 @@
         <v>2</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="53" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="54"/>
+        <v>46</v>
+      </c>
+      <c r="B24" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="58"/>
+      <c r="D24" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="59"/>
       <c r="H24" s="11">
         <v>3</v>
       </c>
@@ -3206,12 +3505,12 @@
         <v>3</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B25" s="1">
         <v>0.25</v>
@@ -3262,12 +3561,12 @@
         <v>4</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B26" s="1">
         <v>0.2</v>
@@ -3283,13 +3582,13 @@
         <f>E25+D26</f>
         <v>0.7</v>
       </c>
-      <c r="S26" s="55" t="s">
-        <v>136</v>
+      <c r="S26" s="37" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B27" s="1">
         <v>0.15</v>
@@ -3305,15 +3604,15 @@
         <f t="shared" ref="E27" si="10">E26+D27</f>
         <v>1</v>
       </c>
-      <c r="H27" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
+      <c r="H27" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1">
         <v>0.2</v>
@@ -3323,18 +3622,18 @@
         <v>0.8</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="40"/>
+        <v>32</v>
+      </c>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B29" s="1">
         <v>0.15</v>
@@ -3344,28 +3643,28 @@
         <v>0.95000000000000007</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H29" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I29" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="I29" s="21" t="s">
-        <v>65</v>
-      </c>
       <c r="J29" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="R29" s="39" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="S29" s="39"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B30" s="1">
         <v>0.05</v>
@@ -3375,10 +3674,10 @@
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H30" s="11">
         <v>1</v>
@@ -3391,7 +3690,7 @@
         <v>1</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
@@ -3409,12 +3708,12 @@
         <v>2</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="39" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
@@ -3433,30 +3732,30 @@
         <v>3</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="S33" s="12" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B34" s="3">
         <v>1</v>
@@ -3470,15 +3769,15 @@
       <c r="E34" s="3">
         <v>0.1</v>
       </c>
-      <c r="H34" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="I34" s="40"/>
-      <c r="J34" s="40"/>
+      <c r="H34" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B35" s="18">
         <v>1</v>
@@ -3492,22 +3791,22 @@
       <c r="E35" s="18">
         <v>1</v>
       </c>
-      <c r="H35" s="40"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="40"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H36" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I36" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="I36" s="21" t="s">
-        <v>65</v>
-      </c>
       <c r="J36" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="R36" s="39" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="S36" s="39"/>
     </row>
@@ -3524,7 +3823,7 @@
         <v>1</v>
       </c>
       <c r="S37" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
@@ -3543,7 +3842,7 @@
         <v>2</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
@@ -3551,15 +3850,15 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G40" s="23"/>
-      <c r="H40" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="I40" s="50"/>
-      <c r="J40" s="38"/>
-      <c r="R40" s="37" t="s">
+      <c r="H40" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="S40" s="38"/>
+      <c r="I40" s="55"/>
+      <c r="J40" s="41"/>
+      <c r="R40" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="S40" s="41"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H41" s="11">
@@ -3575,44 +3874,44 @@
         <v>1</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="H43" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="I43" s="50"/>
-      <c r="J43" s="38"/>
+      <c r="H43" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="I43" s="55"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H44" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I44" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="J44" s="51"/>
-      <c r="K44" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="L44" s="51"/>
-      <c r="M44" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="N44" s="51"/>
-      <c r="O44" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="P44" s="51"/>
+        <v>52</v>
+      </c>
+      <c r="I44" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="J44" s="56"/>
+      <c r="K44" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="L44" s="56"/>
+      <c r="M44" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="N44" s="56"/>
+      <c r="O44" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="P44" s="56"/>
       <c r="R44" s="39" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="S44" s="39"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H45" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I45" s="2">
         <v>0</v>
@@ -3643,15 +3942,15 @@
         <v>0</v>
       </c>
       <c r="R45" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>36</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H46" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I46" s="2">
         <v>0.1</v>
@@ -3682,15 +3981,15 @@
         <v>0.9</v>
       </c>
       <c r="R46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S46" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="S46" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H47" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I47" s="2">
         <v>0.9</v>
@@ -3721,10 +4020,10 @@
         <v>1</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="S47" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="8:16" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Ran ProGenie for 29900 sequences
This updates all files with latest sequences ready to order for
synthesis
</commit_message>
<xml_diff>
--- a/progenieX/ProGenie_Parameters.xlsx
+++ b/progenieX/ProGenie_Parameters.xlsx
@@ -506,22 +506,22 @@
     <t>UAS2_R</t>
   </si>
   <si>
-    <t>TGTGCGGAAGACTT</t>
-  </si>
-  <si>
-    <t>TGGCGAGAAGACCA</t>
-  </si>
-  <si>
-    <t>TCCCCAGAAGACGT</t>
-  </si>
-  <si>
-    <t>TGCGTGGAAGACTA</t>
-  </si>
-  <si>
-    <t>TCTTGCGAAGACTA</t>
-  </si>
-  <si>
-    <t>TGCTGGGAAGACTA</t>
+    <t>TGTGCGGGTCTCATTCT</t>
+  </si>
+  <si>
+    <t>TGGCGAGGTCTCACATT</t>
+  </si>
+  <si>
+    <t>GCCCCAGGTCTCAAAAC</t>
+  </si>
+  <si>
+    <t>TACGTGGGTCTCAGGTC</t>
+  </si>
+  <si>
+    <t>CTCTGTGGTCTCAGTGC</t>
+  </si>
+  <si>
+    <t>TACTCGGGTCTCATCGG</t>
   </si>
 </sst>
 </file>
@@ -892,6 +892,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -901,17 +902,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -931,22 +938,13 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -955,7 +953,9 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1235,7 +1235,7 @@
   <dimension ref="A4:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1243,7 +1243,7 @@
     <col min="1" max="1" width="7.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1251,10 +1251,10 @@
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="39"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -1269,7 +1269,7 @@
       <c r="F5" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="G5" s="39" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       <c r="F6" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G6" s="60" t="s">
+      <c r="G6" s="39" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1303,7 +1303,7 @@
       <c r="F7" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G7" s="60" t="s">
+      <c r="G7" s="39" t="s">
         <v>161</v>
       </c>
       <c r="J7" s="12"/>
@@ -1321,7 +1321,7 @@
       <c r="F8" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="G8" s="60" t="s">
+      <c r="G8" s="39" t="s">
         <v>162</v>
       </c>
     </row>
@@ -1338,7 +1338,7 @@
       <c r="F9" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="G9" s="60" t="s">
+      <c r="G9" s="39" t="s">
         <v>163</v>
       </c>
     </row>
@@ -1355,7 +1355,7 @@
       <c r="F10" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G10" s="60" t="s">
+      <c r="G10" s="39" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1426,18 +1426,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="51" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="49" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1460,11 +1460,11 @@
       <c r="F2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="51"/>
-      <c r="H2" s="46"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="49"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1493,7 +1493,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="45"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
@@ -1520,7 +1520,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1547,7 +1547,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="43" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1567,7 +1567,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="45"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1585,7 +1585,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="45"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1603,7 +1603,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="43" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1623,7 +1623,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="45"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1641,7 +1641,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="45"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1659,7 +1659,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="43" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1679,7 +1679,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="45"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
@@ -1697,7 +1697,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="45"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1715,10 +1715,10 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="50"/>
+      <c r="B16" s="53"/>
       <c r="G16" s="1" t="s">
         <v>93</v>
       </c>
@@ -1739,25 +1739,25 @@
         <v>89</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="40" t="s">
+      <c r="H17" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="I17" s="41"/>
-      <c r="J17" s="40" t="s">
+      <c r="I17" s="42"/>
+      <c r="J17" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="K17" s="41"/>
-      <c r="L17" s="40" t="s">
+      <c r="K17" s="42"/>
+      <c r="L17" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="M17" s="41"/>
-      <c r="N17" s="40" t="s">
+      <c r="M17" s="42"/>
+      <c r="N17" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="O17" s="41"/>
+      <c r="O17" s="42"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="43" t="s">
         <v>88</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1794,13 +1794,13 @@
       <c r="O18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="Q18" s="39" t="s">
+      <c r="Q18" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="R18" s="39"/>
+      <c r="R18" s="40"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="45"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1837,7 +1837,7 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="45"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="1" t="s">
         <v>28</v>
       </c>
@@ -1937,7 +1937,7 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="43" t="s">
         <v>92</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1988,7 +1988,7 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="45"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
@@ -2006,19 +2006,19 @@
       <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="G25" s="40" t="s">
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="G25" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="H25" s="55"/>
-      <c r="I25" s="41"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="42"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="45" t="s">
         <v>139</v>
       </c>
       <c r="B26" s="27">
@@ -2026,25 +2026,25 @@
       </c>
       <c r="C26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="40" t="s">
+      <c r="H26" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="I26" s="41"/>
-      <c r="J26" s="40" t="s">
+      <c r="I26" s="42"/>
+      <c r="J26" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="K26" s="41"/>
-      <c r="L26" s="40" t="s">
+      <c r="K26" s="42"/>
+      <c r="L26" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="M26" s="41"/>
-      <c r="N26" s="40" t="s">
+      <c r="M26" s="42"/>
+      <c r="N26" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="O26" s="41"/>
+      <c r="O26" s="42"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="53"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="1" t="s">
         <v>119</v>
       </c>
@@ -2079,16 +2079,16 @@
       <c r="O27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="Q27" s="40" t="s">
+      <c r="Q27" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="R27" s="41"/>
+      <c r="R27" s="42"/>
       <c r="T27" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="53"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="1" t="s">
         <v>120</v>
       </c>
@@ -2128,7 +2128,7 @@
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" s="53"/>
+      <c r="A29" s="46"/>
       <c r="B29" s="1" t="s">
         <v>121</v>
       </c>
@@ -2181,7 +2181,7 @@
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
+      <c r="A30" s="47"/>
       <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
@@ -2286,26 +2286,26 @@
         <v>0.5</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="40" t="s">
+      <c r="H32" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="I32" s="41"/>
-      <c r="J32" s="40" t="s">
+      <c r="I32" s="42"/>
+      <c r="J32" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="K32" s="41"/>
-      <c r="L32" s="40" t="s">
+      <c r="K32" s="42"/>
+      <c r="L32" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="M32" s="41"/>
-      <c r="N32" s="40" t="s">
+      <c r="M32" s="42"/>
+      <c r="N32" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="O32" s="41"/>
-      <c r="Q32" s="40" t="s">
+      <c r="O32" s="42"/>
+      <c r="Q32" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="R32" s="41"/>
+      <c r="R32" s="42"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="44"/>
@@ -2510,26 +2510,26 @@
       <c r="C39" s="28">
         <v>0.67</v>
       </c>
-      <c r="H39" s="42" t="s">
+      <c r="H39" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="I39" s="43"/>
-      <c r="J39" s="42" t="s">
+      <c r="I39" s="56"/>
+      <c r="J39" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="K39" s="43"/>
-      <c r="L39" s="42" t="s">
+      <c r="K39" s="56"/>
+      <c r="L39" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="M39" s="43"/>
-      <c r="N39" s="42" t="s">
+      <c r="M39" s="56"/>
+      <c r="N39" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="O39" s="43"/>
-      <c r="Q39" s="40" t="s">
+      <c r="O39" s="56"/>
+      <c r="Q39" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="R39" s="41"/>
+      <c r="R39" s="42"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G40" s="1" t="s">
@@ -2613,12 +2613,12 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A44" s="39" t="s">
+      <c r="A44" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
@@ -2654,23 +2654,13 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="A36:A39"/>
     <mergeCell ref="N17:O17"/>
     <mergeCell ref="Q18:R18"/>
     <mergeCell ref="A18:A20"/>
@@ -2683,13 +2673,23 @@
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="Q39:R39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="Q32:R32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2723,23 +2723,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="51" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2754,11 +2754,11 @@
       <c r="D2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="46"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="49"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
@@ -2779,28 +2779,28 @@
       <c r="F3" s="14">
         <v>126</v>
       </c>
-      <c r="H3" s="50" t="s">
+      <c r="H3" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="56" t="s">
+      <c r="I3" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56" t="s">
+      <c r="J3" s="57"/>
+      <c r="K3" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56" t="s">
+      <c r="L3" s="57"/>
+      <c r="M3" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56" t="s">
+      <c r="N3" s="57"/>
+      <c r="O3" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="56"/>
+      <c r="P3" s="57"/>
     </row>
     <row r="4" spans="1:19" ht="33" x14ac:dyDescent="0.3">
-      <c r="H4" s="57"/>
+      <c r="H4" s="60"/>
       <c r="I4" s="21" t="s">
         <v>58</v>
       </c>
@@ -2825,16 +2825,16 @@
       <c r="P4" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="R4" s="39" t="s">
+      <c r="R4" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="S4" s="39"/>
+      <c r="S4" s="40"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="39"/>
+      <c r="B5" s="40"/>
       <c r="H5" s="11">
         <v>1</v>
       </c>
@@ -2862,14 +2862,14 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="39"/>
+      <c r="D6" s="40"/>
       <c r="H6" s="11">
         <v>2</v>
       </c>
@@ -3017,28 +3017,28 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="H10" s="45" t="s">
+      <c r="B10" s="40"/>
+      <c r="H10" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39" t="s">
+      <c r="B11" s="40"/>
+      <c r="C11" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
+      <c r="D11" s="40"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -3053,25 +3053,25 @@
       <c r="D12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="50" t="s">
+      <c r="H12" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="56" t="s">
+      <c r="I12" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56" t="s">
+      <c r="J12" s="57"/>
+      <c r="K12" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56" t="s">
+      <c r="L12" s="57"/>
+      <c r="M12" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="N12" s="56"/>
-      <c r="O12" s="56" t="s">
+      <c r="N12" s="57"/>
+      <c r="O12" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="P12" s="56"/>
+      <c r="P12" s="57"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
@@ -3086,7 +3086,7 @@
       <c r="D13" s="16">
         <v>20</v>
       </c>
-      <c r="H13" s="57"/>
+      <c r="H13" s="60"/>
       <c r="I13" s="21" t="s">
         <v>61</v>
       </c>
@@ -3111,10 +3111,10 @@
       <c r="P13" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="R13" s="39" t="s">
+      <c r="R13" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="S13" s="39"/>
+      <c r="S13" s="40"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
@@ -3276,16 +3276,16 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
-      <c r="H18" s="45" t="s">
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="H18" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
@@ -3301,9 +3301,9 @@
       <c r="E19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -3321,25 +3321,25 @@
       <c r="E20" s="3">
         <v>0.5</v>
       </c>
-      <c r="H20" s="50" t="s">
+      <c r="H20" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="I20" s="56" t="s">
+      <c r="I20" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56" t="s">
+      <c r="J20" s="57"/>
+      <c r="K20" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56" t="s">
+      <c r="L20" s="57"/>
+      <c r="M20" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="N20" s="56"/>
-      <c r="O20" s="56" t="s">
+      <c r="N20" s="57"/>
+      <c r="O20" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="P20" s="56"/>
+      <c r="P20" s="57"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
@@ -3357,7 +3357,7 @@
       <c r="E21" s="18">
         <v>0.1</v>
       </c>
-      <c r="H21" s="57"/>
+      <c r="H21" s="60"/>
       <c r="I21" s="21" t="s">
         <v>61</v>
       </c>
@@ -3382,10 +3382,10 @@
       <c r="P21" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="R21" s="39" t="s">
+      <c r="R21" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="S21" s="39"/>
+      <c r="S21" s="40"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H22" s="11">
@@ -3415,11 +3415,11 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
       <c r="H23" s="11">
         <v>2</v>
       </c>
@@ -3604,11 +3604,11 @@
         <f t="shared" ref="E27" si="10">E26+D27</f>
         <v>1</v>
       </c>
-      <c r="H27" s="45" t="s">
+      <c r="H27" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -3627,9 +3627,9 @@
       <c r="E28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
@@ -3657,10 +3657,10 @@
       <c r="J29" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="R29" s="39" t="s">
+      <c r="R29" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="S29" s="39"/>
+      <c r="S29" s="40"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -3712,12 +3712,12 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
       <c r="H32" s="11">
         <v>3</v>
       </c>
@@ -3769,11 +3769,11 @@
       <c r="E34" s="3">
         <v>0.1</v>
       </c>
-      <c r="H34" s="45" t="s">
+      <c r="H34" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="I34" s="45"/>
-      <c r="J34" s="45"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
@@ -3791,9 +3791,9 @@
       <c r="E35" s="18">
         <v>1</v>
       </c>
-      <c r="H35" s="45"/>
-      <c r="I35" s="45"/>
-      <c r="J35" s="45"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H36" s="19" t="s">
@@ -3805,10 +3805,10 @@
       <c r="J36" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="R36" s="39" t="s">
+      <c r="R36" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="S36" s="39"/>
+      <c r="S36" s="40"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G37" s="22"/>
@@ -3850,15 +3850,15 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G40" s="23"/>
-      <c r="H40" s="40" t="s">
+      <c r="H40" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="I40" s="55"/>
-      <c r="J40" s="41"/>
-      <c r="R40" s="40" t="s">
+      <c r="I40" s="48"/>
+      <c r="J40" s="42"/>
+      <c r="R40" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="S40" s="41"/>
+      <c r="S40" s="42"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H41" s="11">
@@ -3878,36 +3878,36 @@
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="H43" s="40" t="s">
+      <c r="H43" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="I43" s="55"/>
-      <c r="J43" s="41"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="42"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H44" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I44" s="56" t="s">
+      <c r="I44" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="J44" s="56"/>
-      <c r="K44" s="56" t="s">
+      <c r="J44" s="57"/>
+      <c r="K44" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="L44" s="56"/>
-      <c r="M44" s="56" t="s">
+      <c r="L44" s="57"/>
+      <c r="M44" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="N44" s="56"/>
-      <c r="O44" s="56" t="s">
+      <c r="N44" s="57"/>
+      <c r="O44" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="P44" s="56"/>
-      <c r="R44" s="39" t="s">
+      <c r="P44" s="57"/>
+      <c r="R44" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="S44" s="39"/>
+      <c r="S44" s="40"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H45" s="1" t="s">
@@ -4083,27 +4083,17 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="R44:S44"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="R40:S40"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="H18:J19"/>
+    <mergeCell ref="H10:J11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
     <mergeCell ref="H1:J2"/>
     <mergeCell ref="I44:J44"/>
     <mergeCell ref="K44:L44"/>
@@ -4119,17 +4109,27 @@
     <mergeCell ref="H40:J40"/>
     <mergeCell ref="H27:J28"/>
     <mergeCell ref="H34:J35"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="H18:J19"/>
-    <mergeCell ref="H10:J11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="R44:S44"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Consolidation & Record Dictionary
Significant rewrite of code.  Incorporated a dictionary that keeps track
of all changes made to a generated sequence (metadata).
</commit_message>
<xml_diff>
--- a/progenieX/ProGenie_Parameters.xlsx
+++ b/progenieX/ProGenie_Parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15630" windowHeight="7080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15630" windowHeight="7080" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="167">
   <si>
     <t>A</t>
   </si>
@@ -506,22 +506,28 @@
     <t>UAS2_R</t>
   </si>
   <si>
-    <t>TGTGCGGGTCTCATTCT</t>
-  </si>
-  <si>
-    <t>TGGCGAGGTCTCACATT</t>
-  </si>
-  <si>
-    <t>GCCCCAGGTCTCAAAAC</t>
-  </si>
-  <si>
-    <t>TACGTGGGTCTCAGGTC</t>
-  </si>
-  <si>
-    <t>CTCTGTGGTCTCAGTGC</t>
-  </si>
-  <si>
-    <t>TACTCGGGTCTCATCGG</t>
+    <t>TGTGCGGGTCTCA</t>
+  </si>
+  <si>
+    <t>TGGCGAGGTCTCA</t>
+  </si>
+  <si>
+    <t>GCCCCAGGTCTCA</t>
+  </si>
+  <si>
+    <t>TACGTGGGTCTCA</t>
+  </si>
+  <si>
+    <t>CTCTGTGGTCTCA</t>
+  </si>
+  <si>
+    <t>TACTCGGGTCTCA</t>
+  </si>
+  <si>
+    <t># Poly dA:dT to Insert</t>
+  </si>
+  <si>
+    <t>tbp</t>
   </si>
 </sst>
 </file>
@@ -655,7 +661,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -814,11 +820,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -902,23 +917,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -938,13 +947,22 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -953,9 +971,17 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1234,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1404,12 +1430,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9.875" customWidth="1"/>
     <col min="2" max="2" width="9.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.375" customWidth="1"/>
     <col min="7" max="7" width="11.25" customWidth="1"/>
@@ -1426,18 +1453,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="54" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="47" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1460,11 +1487,11 @@
       <c r="F2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="49"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="46" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1493,7 +1520,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="43"/>
+      <c r="A4" s="46"/>
       <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
@@ -1520,7 +1547,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="43"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1547,7 +1574,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="46" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1567,7 +1594,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="43"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1585,7 +1612,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="43"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1603,7 +1630,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="46" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1623,7 +1650,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="43"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1641,7 +1668,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="43"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1659,7 +1686,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="46" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1679,7 +1706,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="43"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
@@ -1697,7 +1724,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="43"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1715,10 +1742,10 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="53"/>
+      <c r="B16" s="51"/>
       <c r="G16" s="1" t="s">
         <v>93</v>
       </c>
@@ -1757,7 +1784,7 @@
       <c r="O17" s="42"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="62" t="s">
         <v>88</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1800,7 +1827,7 @@
       <c r="R18" s="40"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="43"/>
+      <c r="A19" s="63"/>
       <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1837,15 +1864,17 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="43"/>
+      <c r="A20" s="61" t="s">
+        <v>27</v>
+      </c>
       <c r="B20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>32</v>
+      <c r="C20" s="29">
+        <v>15</v>
+      </c>
+      <c r="D20" s="1">
+        <v>15</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>95</v>
@@ -1937,7 +1966,7 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="46" t="s">
         <v>92</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1988,7 +2017,7 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="43"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
@@ -2014,11 +2043,11 @@
       <c r="G25" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="H25" s="48"/>
+      <c r="H25" s="56"/>
       <c r="I25" s="42"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="53" t="s">
         <v>139</v>
       </c>
       <c r="B26" s="27">
@@ -2044,7 +2073,7 @@
       <c r="O26" s="42"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="46"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="1" t="s">
         <v>119</v>
       </c>
@@ -2088,7 +2117,7 @@
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="46"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="1" t="s">
         <v>120</v>
       </c>
@@ -2128,7 +2157,7 @@
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" s="46"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="1" t="s">
         <v>121</v>
       </c>
@@ -2181,7 +2210,7 @@
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A30" s="47"/>
+      <c r="A30" s="55"/>
       <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
@@ -2230,7 +2259,7 @@
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="45" t="s">
         <v>140</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2278,7 +2307,7 @@
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="44"/>
+      <c r="A32" s="45"/>
       <c r="B32" s="1" t="s">
         <v>36</v>
       </c>
@@ -2308,7 +2337,7 @@
       <c r="R32" s="42"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="44"/>
+      <c r="A33" s="45"/>
       <c r="B33" s="1" t="s">
         <v>37</v>
       </c>
@@ -2342,7 +2371,7 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="44"/>
+      <c r="A34" s="45"/>
       <c r="B34" s="1" t="s">
         <v>38</v>
       </c>
@@ -2388,7 +2417,7 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="44"/>
+      <c r="A35" s="45"/>
       <c r="B35" s="2" t="s">
         <v>103</v>
       </c>
@@ -2434,7 +2463,7 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="45" t="s">
         <v>141</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -2482,7 +2511,7 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" s="44"/>
+      <c r="A37" s="45"/>
       <c r="B37" s="2" t="s">
         <v>36</v>
       </c>
@@ -2491,7 +2520,7 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A38" s="44"/>
+      <c r="A38" s="45"/>
       <c r="B38" s="2" t="s">
         <v>37</v>
       </c>
@@ -2503,29 +2532,29 @@
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A39" s="44"/>
+      <c r="A39" s="45"/>
       <c r="B39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="28">
         <v>0.67</v>
       </c>
-      <c r="H39" s="55" t="s">
+      <c r="H39" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="I39" s="56"/>
-      <c r="J39" s="55" t="s">
+      <c r="I39" s="44"/>
+      <c r="J39" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="K39" s="56"/>
-      <c r="L39" s="55" t="s">
+      <c r="K39" s="44"/>
+      <c r="L39" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="M39" s="56"/>
-      <c r="N39" s="55" t="s">
+      <c r="M39" s="44"/>
+      <c r="N39" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="O39" s="56"/>
+      <c r="O39" s="44"/>
       <c r="Q39" s="41" t="s">
         <v>53</v>
       </c>
@@ -2586,6 +2615,12 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A42" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="B42" s="56"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="64"/>
       <c r="G42" s="1" t="s">
         <v>49</v>
       </c>
@@ -2610,6 +2645,14 @@
       </c>
       <c r="R42" s="1" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
@@ -2653,26 +2696,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="Q39:R39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="G1:G2"/>
+  <mergeCells count="37">
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="Q32:R32"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A31:A35"/>
     <mergeCell ref="A26:A30"/>
@@ -2683,13 +2714,26 @@
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="J26:K26"/>
     <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A42:B42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2723,23 +2767,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="54" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2754,11 +2798,11 @@
       <c r="D2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="49"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="47"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
@@ -2779,7 +2823,7 @@
       <c r="F3" s="14">
         <v>126</v>
       </c>
-      <c r="H3" s="53" t="s">
+      <c r="H3" s="51" t="s">
         <v>57</v>
       </c>
       <c r="I3" s="57" t="s">
@@ -2800,7 +2844,7 @@
       <c r="P3" s="57"/>
     </row>
     <row r="4" spans="1:19" ht="33" x14ac:dyDescent="0.3">
-      <c r="H4" s="60"/>
+      <c r="H4" s="58"/>
       <c r="I4" s="21" t="s">
         <v>58</v>
       </c>
@@ -3021,11 +3065,11 @@
         <v>31</v>
       </c>
       <c r="B10" s="40"/>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="40" t="s">
@@ -3036,9 +3080,9 @@
         <v>25</v>
       </c>
       <c r="D11" s="40"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -3053,7 +3097,7 @@
       <c r="D12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="53" t="s">
+      <c r="H12" s="51" t="s">
         <v>57</v>
       </c>
       <c r="I12" s="57" t="s">
@@ -3086,7 +3130,7 @@
       <c r="D13" s="16">
         <v>20</v>
       </c>
-      <c r="H13" s="60"/>
+      <c r="H13" s="58"/>
       <c r="I13" s="21" t="s">
         <v>61</v>
       </c>
@@ -3276,16 +3320,16 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="H18" s="43" t="s">
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="H18" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
@@ -3301,9 +3345,9 @@
       <c r="E19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -3321,7 +3365,7 @@
       <c r="E20" s="3">
         <v>0.5</v>
       </c>
-      <c r="H20" s="53" t="s">
+      <c r="H20" s="51" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="57" t="s">
@@ -3357,7 +3401,7 @@
       <c r="E21" s="18">
         <v>0.1</v>
       </c>
-      <c r="H21" s="60"/>
+      <c r="H21" s="58"/>
       <c r="I21" s="21" t="s">
         <v>61</v>
       </c>
@@ -3462,14 +3506,14 @@
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="58"/>
-      <c r="D24" s="59" t="s">
+      <c r="C24" s="59"/>
+      <c r="D24" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="59"/>
+      <c r="E24" s="60"/>
       <c r="H24" s="11">
         <v>3</v>
       </c>
@@ -3604,11 +3648,11 @@
         <f t="shared" ref="E27" si="10">E26+D27</f>
         <v>1</v>
       </c>
-      <c r="H27" s="43" t="s">
+      <c r="H27" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -3627,9 +3671,9 @@
       <c r="E28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
@@ -3769,11 +3813,11 @@
       <c r="E34" s="3">
         <v>0.1</v>
       </c>
-      <c r="H34" s="43" t="s">
+      <c r="H34" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
@@ -3791,9 +3835,9 @@
       <c r="E35" s="18">
         <v>1</v>
       </c>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="46"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H36" s="19" t="s">
@@ -3853,7 +3897,7 @@
       <c r="H40" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="I40" s="48"/>
+      <c r="I40" s="56"/>
       <c r="J40" s="42"/>
       <c r="R40" s="41" t="s">
         <v>79</v>
@@ -3881,7 +3925,7 @@
       <c r="H43" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="I43" s="48"/>
+      <c r="I43" s="56"/>
       <c r="J43" s="42"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
@@ -4083,17 +4127,27 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="H18:J19"/>
-    <mergeCell ref="H10:J11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="R44:S44"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="R36:S36"/>
     <mergeCell ref="H1:J2"/>
     <mergeCell ref="I44:J44"/>
     <mergeCell ref="K44:L44"/>
@@ -4109,27 +4163,17 @@
     <mergeCell ref="H40:J40"/>
     <mergeCell ref="H27:J28"/>
     <mergeCell ref="H34:J35"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="R44:S44"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="R40:S40"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="R36:S36"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="H18:J19"/>
+    <mergeCell ref="H10:J11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalization & Sequence Creation
Fully extricated all calls to .xlsx into get_data.py.  Added more
functions to separate tasks and for readability.  Created 30K promoter
segments.
</commit_message>
<xml_diff>
--- a/progenieX/ProGenie_Parameters.xlsx
+++ b/progenieX/ProGenie_Parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15630" windowHeight="7080" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15630" windowHeight="7080"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="216">
   <si>
     <t>A</t>
   </si>
@@ -528,6 +528,153 @@
   </si>
   <si>
     <t>tbp</t>
+  </si>
+  <si>
+    <t>NAB3/NRD1 Erase Settings</t>
+  </si>
+  <si>
+    <t>ATG Erase Settings</t>
+  </si>
+  <si>
+    <t>RE Erase Settings</t>
+  </si>
+  <si>
+    <t>Random Sequences (no subs):</t>
+  </si>
+  <si>
+    <t>Number of Sequences:</t>
+  </si>
+  <si>
+    <t>Undesired RE</t>
+  </si>
+  <si>
+    <t>BsaI</t>
+  </si>
+  <si>
+    <t>BbsI</t>
+  </si>
+  <si>
+    <t>SapI</t>
+  </si>
+  <si>
+    <t>MlyI</t>
+  </si>
+  <si>
+    <t>GAAGAC</t>
+  </si>
+  <si>
+    <t>GGTCTC</t>
+  </si>
+  <si>
+    <t>GCTCTTC</t>
+  </si>
+  <si>
+    <t>GAGTC</t>
+  </si>
+  <si>
+    <t>Fix Sequences</t>
+  </si>
+  <si>
+    <t>BbsI_F</t>
+  </si>
+  <si>
+    <t>BsaI_F</t>
+  </si>
+  <si>
+    <t>SapI_F</t>
+  </si>
+  <si>
+    <t>MlyI_F</t>
+  </si>
+  <si>
+    <t>BbsI_R</t>
+  </si>
+  <si>
+    <t>BsaI_R</t>
+  </si>
+  <si>
+    <t>SapI_R</t>
+  </si>
+  <si>
+    <t>MlyI_R</t>
+  </si>
+  <si>
+    <t>GATGAC</t>
+  </si>
+  <si>
+    <t>GTCATC</t>
+  </si>
+  <si>
+    <t>GGTCAC</t>
+  </si>
+  <si>
+    <t>GTGACC</t>
+  </si>
+  <si>
+    <t>GCTCATC</t>
+  </si>
+  <si>
+    <t>GATGAGC</t>
+  </si>
+  <si>
+    <t>GTGTC</t>
+  </si>
+  <si>
+    <t>GACAC</t>
+  </si>
+  <si>
+    <t>Start Codon</t>
+  </si>
+  <si>
+    <t>ATG</t>
+  </si>
+  <si>
+    <t>Fix 2</t>
+  </si>
+  <si>
+    <t>Fix 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix 3 </t>
+  </si>
+  <si>
+    <t>AAG</t>
+  </si>
+  <si>
+    <t>TTG</t>
+  </si>
+  <si>
+    <t>ATC</t>
+  </si>
+  <si>
+    <t>Probability of Fix</t>
+  </si>
+  <si>
+    <t>NAB3</t>
+  </si>
+  <si>
+    <t>NRD1_1</t>
+  </si>
+  <si>
+    <t>NRD1_2</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>Fix</t>
+  </si>
+  <si>
+    <t>TCTT</t>
+  </si>
+  <si>
+    <t>GTAA</t>
+  </si>
+  <si>
+    <t>GTAG</t>
+  </si>
+  <si>
+    <t>GTAT</t>
   </si>
 </sst>
 </file>
@@ -661,7 +808,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -829,11 +976,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -892,9 +1048,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -909,25 +1062,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -941,11 +1093,38 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -956,32 +1135,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1258,29 +1420,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:J16"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="15.25" customWidth="1"/>
     <col min="4" max="6" width="9.5" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="1">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="1">
+        <v>2000</v>
+      </c>
+    </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="40"/>
+      <c r="G4" s="45"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -1289,13 +1469,13 @@
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>145</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="38" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1306,13 +1486,13 @@
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>148</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="38" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1323,13 +1503,13 @@
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>149</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G7" s="39" t="s">
+      <c r="G7" s="38" t="s">
         <v>161</v>
       </c>
       <c r="J7" s="12"/>
@@ -1341,13 +1521,13 @@
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>143</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="38" t="s">
         <v>162</v>
       </c>
     </row>
@@ -1358,13 +1538,13 @@
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>144</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="38" t="s">
         <v>163</v>
       </c>
     </row>
@@ -1375,13 +1555,13 @@
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>146</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="38" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1392,6 +1572,7 @@
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1400,6 +1581,7 @@
       <c r="B12" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="C12" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -1417,9 +1599,243 @@
         <v>12</v>
       </c>
     </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="40"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="44"/>
+      <c r="C19" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="D19" s="45"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D32" s="1">
+        <f>C32</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D33" s="1">
+        <f>C32+C33</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="B36" s="43"/>
+      <c r="C36" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C39" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="9">
     <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1428,10 +1844,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1461,7 +1877,7 @@
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
       <c r="F1" s="50"/>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="53" t="s">
         <v>150</v>
       </c>
       <c r="H1" s="47" t="s">
@@ -1487,11 +1903,11 @@
       <c r="F2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="52"/>
+      <c r="G2" s="53"/>
       <c r="H2" s="47"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="51" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1520,7 +1936,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="46"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
@@ -1547,7 +1963,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1574,7 +1990,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="51" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1594,7 +2010,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
@@ -1612,7 +2028,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1630,7 +2046,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="51" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1650,7 +2066,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1668,7 +2084,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="46"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1686,7 +2102,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="51" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1706,7 +2122,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="46"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
@@ -1724,7 +2140,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="46"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1742,10 +2158,10 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="51"/>
+      <c r="B16" s="52"/>
       <c r="G16" s="1" t="s">
         <v>93</v>
       </c>
@@ -1766,25 +2182,25 @@
         <v>89</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="41" t="s">
+      <c r="H17" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="I17" s="42"/>
-      <c r="J17" s="41" t="s">
+      <c r="I17" s="43"/>
+      <c r="J17" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="K17" s="42"/>
-      <c r="L17" s="41" t="s">
+      <c r="K17" s="43"/>
+      <c r="L17" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="M17" s="42"/>
-      <c r="N17" s="41" t="s">
+      <c r="M17" s="43"/>
+      <c r="N17" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="O17" s="42"/>
+      <c r="O17" s="43"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="54" t="s">
         <v>88</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1821,21 +2237,21 @@
       <c r="O18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="Q18" s="40" t="s">
+      <c r="Q18" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="R18" s="40"/>
+      <c r="R18" s="45"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="63"/>
+      <c r="A19" s="55"/>
       <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>32</v>
+      <c r="C19" s="29">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>94</v>
@@ -1864,17 +2280,15 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="61" t="s">
-        <v>27</v>
-      </c>
+      <c r="A20" s="56"/>
       <c r="B20" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="29">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D20" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>95</v>
@@ -1915,7 +2329,7 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="34" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1966,7 +2380,7 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="51" t="s">
         <v>92</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2017,37 +2431,45 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="46"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>32</v>
+      <c r="C23" s="29">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="30"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
+      <c r="A24" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="29">
+        <v>15</v>
+      </c>
+      <c r="D24" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="G25" s="41" t="s">
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="G25" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="H25" s="56"/>
-      <c r="I25" s="42"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="43"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="53" t="s">
+      <c r="A26" s="62" t="s">
         <v>139</v>
       </c>
       <c r="B26" s="27">
@@ -2055,25 +2477,25 @@
       </c>
       <c r="C26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="41" t="s">
+      <c r="H26" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="I26" s="42"/>
-      <c r="J26" s="41" t="s">
+      <c r="I26" s="43"/>
+      <c r="J26" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="K26" s="42"/>
-      <c r="L26" s="41" t="s">
+      <c r="K26" s="43"/>
+      <c r="L26" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="M26" s="42"/>
-      <c r="N26" s="41" t="s">
+      <c r="M26" s="43"/>
+      <c r="N26" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="O26" s="42"/>
+      <c r="O26" s="43"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
+      <c r="A27" s="63"/>
       <c r="B27" s="1" t="s">
         <v>119</v>
       </c>
@@ -2108,16 +2530,16 @@
       <c r="O27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="Q27" s="41" t="s">
+      <c r="Q27" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="R27" s="42"/>
+      <c r="R27" s="43"/>
       <c r="T27" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
+      <c r="A28" s="63"/>
       <c r="B28" s="1" t="s">
         <v>120</v>
       </c>
@@ -2157,7 +2579,7 @@
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
+      <c r="A29" s="63"/>
       <c r="B29" s="1" t="s">
         <v>121</v>
       </c>
@@ -2174,28 +2596,28 @@
       <c r="H29" s="1">
         <v>0.33</v>
       </c>
-      <c r="I29" s="31">
+      <c r="I29" s="30">
         <f>H29</f>
         <v>0.33</v>
       </c>
       <c r="J29" s="1">
         <v>0.3</v>
       </c>
-      <c r="K29" s="31">
+      <c r="K29" s="30">
         <f>J29</f>
         <v>0.3</v>
       </c>
       <c r="L29" s="1">
         <v>0.25</v>
       </c>
-      <c r="M29" s="31">
+      <c r="M29" s="30">
         <f>L29</f>
         <v>0.25</v>
       </c>
       <c r="N29" s="1">
         <v>0.1</v>
       </c>
-      <c r="O29" s="31">
+      <c r="O29" s="30">
         <f>N29</f>
         <v>0.1</v>
       </c>
@@ -2210,11 +2632,11 @@
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A30" s="55"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="30" t="s">
         <v>137</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -2223,28 +2645,28 @@
       <c r="H30" s="1">
         <v>0.33</v>
       </c>
-      <c r="I30" s="31">
+      <c r="I30" s="30">
         <f>I29+H30</f>
         <v>0.66</v>
       </c>
       <c r="J30" s="1">
         <v>0.3</v>
       </c>
-      <c r="K30" s="31">
+      <c r="K30" s="30">
         <f>K29+J30</f>
         <v>0.6</v>
       </c>
       <c r="L30" s="1">
         <v>0.25</v>
       </c>
-      <c r="M30" s="31">
+      <c r="M30" s="30">
         <f>M29+L30</f>
         <v>0.5</v>
       </c>
       <c r="N30" s="1">
         <v>0.1</v>
       </c>
-      <c r="O30" s="31">
+      <c r="O30" s="30">
         <f>O29+N30</f>
         <v>0.2</v>
       </c>
@@ -2259,7 +2681,7 @@
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="61" t="s">
         <v>140</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2274,28 +2696,28 @@
       <c r="H31" s="1">
         <v>0</v>
       </c>
-      <c r="I31" s="31">
+      <c r="I31" s="30">
         <f>I30+H31</f>
         <v>0.66</v>
       </c>
       <c r="J31" s="1">
         <v>0.1</v>
       </c>
-      <c r="K31" s="31">
+      <c r="K31" s="30">
         <f>K30+J31</f>
         <v>0.7</v>
       </c>
       <c r="L31" s="1">
         <v>0.25</v>
       </c>
-      <c r="M31" s="31">
+      <c r="M31" s="30">
         <f>M30+L31</f>
         <v>0.75</v>
       </c>
       <c r="N31" s="1">
         <v>0.7</v>
       </c>
-      <c r="O31" s="31">
+      <c r="O31" s="30">
         <f>O30+N31</f>
         <v>0.89999999999999991</v>
       </c>
@@ -2307,7 +2729,7 @@
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="45"/>
+      <c r="A32" s="61"/>
       <c r="B32" s="1" t="s">
         <v>36</v>
       </c>
@@ -2315,29 +2737,29 @@
         <v>0.5</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="41" t="s">
+      <c r="H32" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="I32" s="42"/>
-      <c r="J32" s="41" t="s">
+      <c r="I32" s="43"/>
+      <c r="J32" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="K32" s="42"/>
-      <c r="L32" s="41" t="s">
+      <c r="K32" s="43"/>
+      <c r="L32" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="M32" s="42"/>
-      <c r="N32" s="41" t="s">
+      <c r="M32" s="43"/>
+      <c r="N32" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="O32" s="42"/>
-      <c r="Q32" s="41" t="s">
+      <c r="O32" s="43"/>
+      <c r="Q32" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="R32" s="42"/>
+      <c r="R32" s="43"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="45"/>
+      <c r="A33" s="61"/>
       <c r="B33" s="1" t="s">
         <v>37</v>
       </c>
@@ -2371,7 +2793,7 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="45"/>
+      <c r="A34" s="61"/>
       <c r="B34" s="1" t="s">
         <v>38</v>
       </c>
@@ -2384,28 +2806,28 @@
       <c r="H34" s="1">
         <v>0.5</v>
       </c>
-      <c r="I34" s="32">
+      <c r="I34" s="31">
         <f>H34</f>
         <v>0.5</v>
       </c>
       <c r="J34" s="1">
         <v>0.4</v>
       </c>
-      <c r="K34" s="32">
+      <c r="K34" s="31">
         <f>J34</f>
         <v>0.4</v>
       </c>
       <c r="L34" s="1">
         <v>0.25</v>
       </c>
-      <c r="M34" s="32">
+      <c r="M34" s="31">
         <f>L34</f>
         <v>0.25</v>
       </c>
       <c r="N34" s="1">
         <v>0.1</v>
       </c>
-      <c r="O34" s="32">
+      <c r="O34" s="31">
         <f>N34</f>
         <v>0.1</v>
       </c>
@@ -2417,7 +2839,7 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
+      <c r="A35" s="61"/>
       <c r="B35" s="2" t="s">
         <v>103</v>
       </c>
@@ -2430,28 +2852,28 @@
       <c r="H35" s="1">
         <v>0</v>
       </c>
-      <c r="I35" s="32">
+      <c r="I35" s="31">
         <f>I34+H35</f>
         <v>0.5</v>
       </c>
       <c r="J35" s="1">
         <v>0.1</v>
       </c>
-      <c r="K35" s="32">
+      <c r="K35" s="31">
         <f>K34+J35</f>
         <v>0.5</v>
       </c>
       <c r="L35" s="1">
         <v>0.25</v>
       </c>
-      <c r="M35" s="32">
+      <c r="M35" s="31">
         <f>M34+L35</f>
         <v>0.5</v>
       </c>
       <c r="N35" s="1">
         <v>0.4</v>
       </c>
-      <c r="O35" s="32">
+      <c r="O35" s="31">
         <f>O34+N35</f>
         <v>0.5</v>
       </c>
@@ -2463,7 +2885,7 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="61" t="s">
         <v>141</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -2478,28 +2900,28 @@
       <c r="H36" s="1">
         <v>0</v>
       </c>
-      <c r="I36" s="32">
+      <c r="I36" s="31">
         <f>I35+H36</f>
         <v>0.5</v>
       </c>
       <c r="J36" s="1">
         <v>0.1</v>
       </c>
-      <c r="K36" s="32">
+      <c r="K36" s="31">
         <f>K35+J36</f>
         <v>0.6</v>
       </c>
       <c r="L36" s="1">
         <v>0.25</v>
       </c>
-      <c r="M36" s="32">
+      <c r="M36" s="31">
         <f>M35+L36</f>
         <v>0.75</v>
       </c>
       <c r="N36" s="1">
         <v>0.4</v>
       </c>
-      <c r="O36" s="32">
+      <c r="O36" s="31">
         <f>O35+N36</f>
         <v>0.9</v>
       </c>
@@ -2511,7 +2933,7 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" s="45"/>
+      <c r="A37" s="61"/>
       <c r="B37" s="2" t="s">
         <v>36</v>
       </c>
@@ -2520,45 +2942,50 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A38" s="45"/>
+      <c r="A38" s="61"/>
       <c r="B38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="28">
         <v>0.25</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="42" t="s">
         <v>128</v>
       </c>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="43"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A39" s="45"/>
+      <c r="A39" s="61"/>
       <c r="B39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="28">
         <v>0.67</v>
       </c>
-      <c r="H39" s="43" t="s">
+      <c r="G39" s="1"/>
+      <c r="H39" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="I39" s="44"/>
-      <c r="J39" s="43" t="s">
+      <c r="I39" s="58"/>
+      <c r="J39" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="K39" s="44"/>
-      <c r="L39" s="43" t="s">
+      <c r="K39" s="58"/>
+      <c r="L39" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="M39" s="44"/>
-      <c r="N39" s="43" t="s">
+      <c r="M39" s="60"/>
+      <c r="N39" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="O39" s="44"/>
-      <c r="Q39" s="41" t="s">
+      <c r="O39" s="60"/>
+      <c r="Q39" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="R39" s="42"/>
+      <c r="R39" s="43"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G40" s="1" t="s">
@@ -2591,22 +3018,22 @@
       <c r="G41" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H41" s="38">
+      <c r="H41" s="37">
         <v>0.25</v>
       </c>
-      <c r="I41" s="38"/>
-      <c r="J41" s="38">
-        <v>0.5</v>
-      </c>
-      <c r="K41" s="38"/>
-      <c r="L41" s="38">
+      <c r="I41" s="37"/>
+      <c r="J41" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="K41" s="37"/>
+      <c r="L41" s="37">
         <v>0.75</v>
       </c>
-      <c r="M41" s="38"/>
-      <c r="N41" s="38">
+      <c r="M41" s="37"/>
+      <c r="N41" s="37">
         <v>0.9</v>
       </c>
-      <c r="O41" s="38"/>
+      <c r="O41" s="37"/>
       <c r="Q41" s="1" t="s">
         <v>51</v>
       </c>
@@ -2615,31 +3042,31 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="65"/>
-      <c r="D42" s="64"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="40"/>
       <c r="G42" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H42" s="38">
+      <c r="H42" s="37">
         <v>0.75</v>
       </c>
-      <c r="I42" s="38"/>
-      <c r="J42" s="38">
-        <v>0.5</v>
-      </c>
-      <c r="K42" s="38"/>
-      <c r="L42" s="38">
+      <c r="I42" s="37"/>
+      <c r="J42" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37">
         <v>0.25</v>
       </c>
-      <c r="M42" s="38"/>
-      <c r="N42" s="38">
+      <c r="M42" s="37"/>
+      <c r="N42" s="37">
         <v>0.1</v>
       </c>
-      <c r="O42" s="38"/>
+      <c r="O42" s="37"/>
       <c r="Q42" s="1" t="s">
         <v>49</v>
       </c>
@@ -2656,12 +3083,17 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A44" s="40" t="s">
+      <c r="A44" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="40"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="40"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
@@ -2671,12 +3103,17 @@
       <c r="C45" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D45" s="36" t="s">
+      <c r="D45" s="35" t="s">
         <v>37</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="23"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
@@ -2694,27 +3131,67 @@
       <c r="E46" s="3">
         <v>0.1</v>
       </c>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="23"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G47" s="23"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="23"/>
+      <c r="K47" s="23"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="23"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="B49" s="46"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="43"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="40"/>
+      <c r="J49" s="40"/>
+      <c r="K49" s="40"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="B54" s="46"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="Q32:R32"/>
+  <mergeCells count="40">
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="G38:K38"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A31:A35"/>
     <mergeCell ref="A26:A30"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
     <mergeCell ref="A25:C25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="A18:A19"/>
     <mergeCell ref="N17:O17"/>
     <mergeCell ref="Q18:R18"/>
     <mergeCell ref="H1:H2"/>
@@ -2726,14 +3203,19 @@
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="Q39:R39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="Q32:R32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2773,17 +3255,17 @@
       <c r="B1" s="47"/>
       <c r="C1" s="47"/>
       <c r="D1" s="47"/>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="53" t="s">
         <v>21</v>
       </c>
       <c r="F1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2798,11 +3280,11 @@
       <c r="D2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="52"/>
+      <c r="E2" s="53"/>
       <c r="F2" s="47"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
@@ -2823,28 +3305,28 @@
       <c r="F3" s="14">
         <v>126</v>
       </c>
-      <c r="H3" s="51" t="s">
+      <c r="H3" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="57" t="s">
+      <c r="I3" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57" t="s">
+      <c r="J3" s="44"/>
+      <c r="K3" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57" t="s">
+      <c r="L3" s="44"/>
+      <c r="M3" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57" t="s">
+      <c r="N3" s="44"/>
+      <c r="O3" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="57"/>
+      <c r="P3" s="44"/>
     </row>
     <row r="4" spans="1:19" ht="33" x14ac:dyDescent="0.3">
-      <c r="H4" s="58"/>
+      <c r="H4" s="67"/>
       <c r="I4" s="21" t="s">
         <v>58</v>
       </c>
@@ -2869,16 +3351,16 @@
       <c r="P4" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="R4" s="40" t="s">
+      <c r="R4" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="S4" s="40"/>
+      <c r="S4" s="45"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="40"/>
+      <c r="B5" s="45"/>
       <c r="H5" s="11">
         <v>1</v>
       </c>
@@ -2906,14 +3388,14 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40" t="s">
+      <c r="B6" s="45"/>
+      <c r="C6" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="40"/>
+      <c r="D6" s="45"/>
       <c r="H6" s="11">
         <v>2</v>
       </c>
@@ -3056,33 +3538,33 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="S9" s="37" t="s">
+      <c r="S9" s="36" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="H10" s="46" t="s">
+      <c r="B10" s="45"/>
+      <c r="H10" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40" t="s">
+      <c r="B11" s="45"/>
+      <c r="C11" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
+      <c r="D11" s="45"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -3097,25 +3579,25 @@
       <c r="D12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="51" t="s">
+      <c r="H12" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="57" t="s">
+      <c r="I12" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57" t="s">
+      <c r="J12" s="44"/>
+      <c r="K12" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57" t="s">
+      <c r="L12" s="44"/>
+      <c r="M12" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="N12" s="57"/>
-      <c r="O12" s="57" t="s">
+      <c r="N12" s="44"/>
+      <c r="O12" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="P12" s="57"/>
+      <c r="P12" s="44"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
@@ -3130,7 +3612,7 @@
       <c r="D13" s="16">
         <v>20</v>
       </c>
-      <c r="H13" s="58"/>
+      <c r="H13" s="67"/>
       <c r="I13" s="21" t="s">
         <v>61</v>
       </c>
@@ -3155,10 +3637,10 @@
       <c r="P13" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="R13" s="40" t="s">
+      <c r="R13" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="S13" s="40"/>
+      <c r="S13" s="45"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
@@ -3257,7 +3739,7 @@
       <c r="A16" s="17">
         <v>0</v>
       </c>
-      <c r="B16" s="36">
+      <c r="B16" s="35">
         <v>0</v>
       </c>
       <c r="C16" s="15">
@@ -3315,21 +3797,21 @@
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="R17" s="12"/>
-      <c r="S17" s="37" t="s">
+      <c r="S17" s="36" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="H18" s="46" t="s">
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="H18" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
@@ -3345,9 +3827,9 @@
       <c r="E19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -3365,25 +3847,25 @@
       <c r="E20" s="3">
         <v>0.5</v>
       </c>
-      <c r="H20" s="51" t="s">
+      <c r="H20" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="I20" s="57" t="s">
+      <c r="I20" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57" t="s">
+      <c r="J20" s="44"/>
+      <c r="K20" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="L20" s="57"/>
-      <c r="M20" s="57" t="s">
+      <c r="L20" s="44"/>
+      <c r="M20" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="N20" s="57"/>
-      <c r="O20" s="57" t="s">
+      <c r="N20" s="44"/>
+      <c r="O20" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="P20" s="57"/>
+      <c r="P20" s="44"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
@@ -3401,7 +3883,7 @@
       <c r="E21" s="18">
         <v>0.1</v>
       </c>
-      <c r="H21" s="58"/>
+      <c r="H21" s="67"/>
       <c r="I21" s="21" t="s">
         <v>61</v>
       </c>
@@ -3426,10 +3908,10 @@
       <c r="P21" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="R21" s="40" t="s">
+      <c r="R21" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="S21" s="40"/>
+      <c r="S21" s="45"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H22" s="11">
@@ -3459,11 +3941,11 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
       <c r="H23" s="11">
         <v>2</v>
       </c>
@@ -3506,14 +3988,14 @@
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="60" t="s">
+      <c r="C24" s="65"/>
+      <c r="D24" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="60"/>
+      <c r="E24" s="66"/>
       <c r="H24" s="11">
         <v>3</v>
       </c>
@@ -3626,7 +4108,7 @@
         <f>E25+D26</f>
         <v>0.7</v>
       </c>
-      <c r="S26" s="37" t="s">
+      <c r="S26" s="36" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3648,11 +4130,11 @@
         <f t="shared" ref="E27" si="10">E26+D27</f>
         <v>1</v>
       </c>
-      <c r="H27" s="46" t="s">
+      <c r="H27" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -3671,9 +4153,9 @@
       <c r="E28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H28" s="46"/>
-      <c r="I28" s="46"/>
-      <c r="J28" s="46"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
@@ -3701,10 +4183,10 @@
       <c r="J29" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="R29" s="40" t="s">
+      <c r="R29" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="S29" s="40"/>
+      <c r="S29" s="45"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -3756,12 +4238,12 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
       <c r="H32" s="11">
         <v>3</v>
       </c>
@@ -3813,11 +4295,11 @@
       <c r="E34" s="3">
         <v>0.1</v>
       </c>
-      <c r="H34" s="46" t="s">
+      <c r="H34" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="I34" s="46"/>
-      <c r="J34" s="46"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="51"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
@@ -3835,9 +4317,9 @@
       <c r="E35" s="18">
         <v>1</v>
       </c>
-      <c r="H35" s="46"/>
-      <c r="I35" s="46"/>
-      <c r="J35" s="46"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="51"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H36" s="19" t="s">
@@ -3849,10 +4331,10 @@
       <c r="J36" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="R36" s="40" t="s">
+      <c r="R36" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="S36" s="40"/>
+      <c r="S36" s="45"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G37" s="22"/>
@@ -3894,15 +4376,15 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="G40" s="23"/>
-      <c r="H40" s="41" t="s">
+      <c r="H40" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="I40" s="56"/>
-      <c r="J40" s="42"/>
-      <c r="R40" s="41" t="s">
+      <c r="I40" s="46"/>
+      <c r="J40" s="43"/>
+      <c r="R40" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="S40" s="42"/>
+      <c r="S40" s="43"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H41" s="11">
@@ -3922,36 +4404,36 @@
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="H43" s="41" t="s">
+      <c r="H43" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="I43" s="56"/>
-      <c r="J43" s="42"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H44" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I44" s="57" t="s">
+      <c r="I44" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="J44" s="57"/>
-      <c r="K44" s="57" t="s">
+      <c r="J44" s="44"/>
+      <c r="K44" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="L44" s="57"/>
-      <c r="M44" s="57" t="s">
+      <c r="L44" s="44"/>
+      <c r="M44" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="N44" s="57"/>
-      <c r="O44" s="57" t="s">
+      <c r="N44" s="44"/>
+      <c r="O44" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="P44" s="57"/>
-      <c r="R44" s="40" t="s">
+      <c r="P44" s="44"/>
+      <c r="R44" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="S44" s="40"/>
+      <c r="S44" s="45"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H45" s="1" t="s">
@@ -4071,83 +4553,73 @@
       </c>
     </row>
     <row r="49" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H49" s="34"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="34"/>
-      <c r="K49" s="33"/>
-      <c r="L49" s="33"/>
-      <c r="M49" s="33"/>
-      <c r="N49" s="33"/>
-      <c r="O49" s="33"/>
-      <c r="P49" s="33"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="33"/>
+      <c r="K49" s="32"/>
+      <c r="L49" s="32"/>
+      <c r="M49" s="32"/>
+      <c r="N49" s="32"/>
+      <c r="O49" s="32"/>
+      <c r="P49" s="32"/>
     </row>
     <row r="50" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H50" s="33"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="34"/>
-      <c r="K50" s="34"/>
-      <c r="L50" s="34"/>
-      <c r="M50" s="34"/>
-      <c r="N50" s="34"/>
-      <c r="O50" s="34"/>
-      <c r="P50" s="34"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="33"/>
+      <c r="K50" s="33"/>
+      <c r="L50" s="33"/>
+      <c r="M50" s="33"/>
+      <c r="N50" s="33"/>
+      <c r="O50" s="33"/>
+      <c r="P50" s="33"/>
     </row>
     <row r="51" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H51" s="33"/>
-      <c r="I51" s="33"/>
-      <c r="J51" s="33"/>
-      <c r="K51" s="33"/>
-      <c r="L51" s="33"/>
-      <c r="M51" s="33"/>
-      <c r="N51" s="33"/>
-      <c r="O51" s="33"/>
-      <c r="P51" s="33"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="32"/>
+      <c r="L51" s="32"/>
+      <c r="M51" s="32"/>
+      <c r="N51" s="32"/>
+      <c r="O51" s="32"/>
+      <c r="P51" s="32"/>
     </row>
     <row r="52" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H52" s="33"/>
-      <c r="I52" s="33"/>
-      <c r="J52" s="33"/>
-      <c r="K52" s="33"/>
-      <c r="L52" s="33"/>
-      <c r="M52" s="33"/>
-      <c r="N52" s="33"/>
-      <c r="O52" s="33"/>
-      <c r="P52" s="33"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
+      <c r="J52" s="32"/>
+      <c r="K52" s="32"/>
+      <c r="L52" s="32"/>
+      <c r="M52" s="32"/>
+      <c r="N52" s="32"/>
+      <c r="O52" s="32"/>
+      <c r="P52" s="32"/>
     </row>
     <row r="53" spans="8:16" x14ac:dyDescent="0.3">
-      <c r="H53" s="33"/>
-      <c r="I53" s="33"/>
-      <c r="J53" s="33"/>
-      <c r="K53" s="33"/>
-      <c r="L53" s="33"/>
-      <c r="M53" s="33"/>
-      <c r="N53" s="33"/>
-      <c r="O53" s="33"/>
-      <c r="P53" s="33"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32"/>
+      <c r="J53" s="32"/>
+      <c r="K53" s="32"/>
+      <c r="L53" s="32"/>
+      <c r="M53" s="32"/>
+      <c r="N53" s="32"/>
+      <c r="O53" s="32"/>
+      <c r="P53" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="R44:S44"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="R40:S40"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="H18:J19"/>
+    <mergeCell ref="H10:J11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
     <mergeCell ref="H1:J2"/>
     <mergeCell ref="I44:J44"/>
     <mergeCell ref="K44:L44"/>
@@ -4163,17 +4635,27 @@
     <mergeCell ref="H40:J40"/>
     <mergeCell ref="H27:J28"/>
     <mergeCell ref="H34:J35"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="H18:J19"/>
-    <mergeCell ref="H10:J11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="R44:S44"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>